<commit_message>
Finished file that records and writes to excel the return during the first 30 min of the day Last step is to write code the find return during the last 30 min of the day Then have the files run for some time: During this Time I can see if I can find historical data to use instead
</commit_message>
<xml_diff>
--- a/calls_output.xlsx
+++ b/calls_output.xlsx
@@ -587,18 +587,14 @@
       <c r="P2" t="n">
         <v>1</v>
       </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="T2" t="n">
-        <v>-0.055</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -657,18 +653,14 @@
       <c r="P3" t="n">
         <v>1</v>
       </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="n">
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0.011</v>
-      </c>
-      <c r="T3" t="n">
-        <v>-0.056</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -727,18 +719,14 @@
       <c r="P4" t="n">
         <v>1</v>
       </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q4" t="inlineStr"/>
       <c r="R4" t="n">
         <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>0.011</v>
-      </c>
-      <c r="T4" t="n">
-        <v>-0.058</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -797,18 +785,14 @@
       <c r="P5" t="n">
         <v>1</v>
       </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q5" t="inlineStr"/>
       <c r="R5" t="n">
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>0.011</v>
-      </c>
-      <c r="T5" t="n">
-        <v>-0.059</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -867,18 +851,14 @@
       <c r="P6" t="n">
         <v>1</v>
       </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q6" t="inlineStr"/>
       <c r="R6" t="n">
         <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="T6" t="n">
-        <v>-0.06</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -937,18 +917,14 @@
       <c r="P7" t="n">
         <v>1</v>
       </c>
-      <c r="Q7" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="T7" t="n">
-        <v>-0.061</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1007,18 +983,14 @@
       <c r="P8" t="n">
         <v>1</v>
       </c>
-      <c r="Q8" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="n">
         <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="T8" t="n">
-        <v>-0.061</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1077,18 +1049,14 @@
       <c r="P9" t="n">
         <v>1</v>
       </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q9" t="inlineStr"/>
       <c r="R9" t="n">
         <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="T9" t="n">
-        <v>-0.062</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1147,18 +1115,14 @@
       <c r="P10" t="n">
         <v>1</v>
       </c>
-      <c r="Q10" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q10" t="inlineStr"/>
       <c r="R10" t="n">
         <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="T10" t="n">
-        <v>-0.062</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1217,18 +1181,14 @@
       <c r="P11" t="n">
         <v>1</v>
       </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
         <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="T11" t="n">
-        <v>-0.062</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1287,18 +1247,14 @@
       <c r="P12" t="n">
         <v>1</v>
       </c>
-      <c r="Q12" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q12" t="inlineStr"/>
       <c r="R12" t="n">
         <v>0</v>
       </c>
       <c r="S12" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="T12" t="n">
-        <v>-0.062</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1357,18 +1313,14 @@
       <c r="P13" t="n">
         <v>1</v>
       </c>
-      <c r="Q13" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q13" t="inlineStr"/>
       <c r="R13" t="n">
         <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="T13" t="n">
-        <v>-0.062</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1427,18 +1379,14 @@
       <c r="P14" t="n">
         <v>1</v>
       </c>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q14" t="inlineStr"/>
       <c r="R14" t="n">
         <v>0</v>
       </c>
       <c r="S14" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="T14" t="n">
-        <v>-0.062</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1497,18 +1445,14 @@
       <c r="P15" t="n">
         <v>1</v>
       </c>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q15" t="inlineStr"/>
       <c r="R15" t="n">
         <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="T15" t="n">
-        <v>-0.062</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1567,18 +1511,14 @@
       <c r="P16" t="n">
         <v>1</v>
       </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="n">
         <v>0</v>
       </c>
       <c r="S16" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="T16" t="n">
-        <v>-0.063</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1637,18 +1577,14 @@
       <c r="P17" t="n">
         <v>1</v>
       </c>
-      <c r="Q17" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q17" t="inlineStr"/>
       <c r="R17" t="n">
         <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="T17" t="n">
-        <v>-0.063</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1705,20 +1641,16 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0.021</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q18" t="inlineStr"/>
       <c r="R18" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
       </c>
-      <c r="T18" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1777,18 +1709,14 @@
       <c r="P19" t="n">
         <v>0</v>
       </c>
-      <c r="Q19" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q19" t="inlineStr"/>
       <c r="R19" t="n">
         <v>0</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
       </c>
-      <c r="T19" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1847,18 +1775,14 @@
       <c r="P20" t="n">
         <v>0</v>
       </c>
-      <c r="Q20" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="Q20" t="inlineStr"/>
       <c r="R20" t="n">
         <v>0</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
       </c>
-      <c r="T20" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1917,18 +1841,14 @@
       <c r="P21" t="n">
         <v>0</v>
       </c>
-      <c r="Q21" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q21" t="inlineStr"/>
       <c r="R21" t="n">
         <v>0</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
       </c>
-      <c r="T21" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1985,20 +1905,16 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>0.002</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q22" t="inlineStr"/>
       <c r="R22" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="S22" t="n">
         <v>0</v>
       </c>
-      <c r="T22" t="n">
-        <v>-0.002</v>
-      </c>
+      <c r="T22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2057,18 +1973,14 @@
       <c r="P23" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q23" t="inlineStr"/>
       <c r="R23" t="n">
         <v>0</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
       </c>
-      <c r="T23" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2127,18 +2039,14 @@
       <c r="P24" t="n">
         <v>0</v>
       </c>
-      <c r="Q24" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q24" t="inlineStr"/>
       <c r="R24" t="n">
         <v>0</v>
       </c>
       <c r="S24" t="n">
         <v>0</v>
       </c>
-      <c r="T24" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2197,18 +2105,14 @@
       <c r="P25" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q25" t="inlineStr"/>
       <c r="R25" t="n">
         <v>0</v>
       </c>
       <c r="S25" t="n">
         <v>0</v>
       </c>
-      <c r="T25" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2267,18 +2171,14 @@
       <c r="P26" t="n">
         <v>0</v>
       </c>
-      <c r="Q26" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q26" t="inlineStr"/>
       <c r="R26" t="n">
         <v>0</v>
       </c>
       <c r="S26" t="n">
         <v>0</v>
       </c>
-      <c r="T26" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2337,18 +2237,14 @@
       <c r="P27" t="n">
         <v>0</v>
       </c>
-      <c r="Q27" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="Q27" t="inlineStr"/>
       <c r="R27" t="n">
         <v>0</v>
       </c>
       <c r="S27" t="n">
         <v>0</v>
       </c>
-      <c r="T27" t="n">
-        <v>-0.002</v>
-      </c>
+      <c r="T27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2407,18 +2303,14 @@
       <c r="P28" t="n">
         <v>0</v>
       </c>
-      <c r="Q28" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q28" t="inlineStr"/>
       <c r="R28" t="n">
         <v>0</v>
       </c>
       <c r="S28" t="n">
         <v>0</v>
       </c>
-      <c r="T28" t="n">
-        <v>-0.001</v>
-      </c>
+      <c r="T28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2477,18 +2369,14 @@
       <c r="P29" t="n">
         <v>0</v>
       </c>
-      <c r="Q29" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q29" t="inlineStr"/>
       <c r="R29" t="n">
         <v>0</v>
       </c>
       <c r="S29" t="n">
         <v>0</v>
       </c>
-      <c r="T29" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2547,18 +2435,14 @@
       <c r="P30" t="n">
         <v>0</v>
       </c>
-      <c r="Q30" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q30" t="inlineStr"/>
       <c r="R30" t="n">
         <v>0</v>
       </c>
       <c r="S30" t="n">
         <v>0</v>
       </c>
-      <c r="T30" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -2617,18 +2501,14 @@
       <c r="P31" t="n">
         <v>0</v>
       </c>
-      <c r="Q31" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q31" t="inlineStr"/>
       <c r="R31" t="n">
         <v>0</v>
       </c>
       <c r="S31" t="n">
         <v>0</v>
       </c>
-      <c r="T31" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -2687,18 +2567,14 @@
       <c r="P32" t="n">
         <v>0</v>
       </c>
-      <c r="Q32" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q32" t="inlineStr"/>
       <c r="R32" t="n">
         <v>0</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
       </c>
-      <c r="T32" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -2757,18 +2633,14 @@
       <c r="P33" t="n">
         <v>0</v>
       </c>
-      <c r="Q33" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q33" t="inlineStr"/>
       <c r="R33" t="n">
         <v>0</v>
       </c>
       <c r="S33" t="n">
         <v>0</v>
       </c>
-      <c r="T33" t="n">
-        <v>-0.004</v>
-      </c>
+      <c r="T33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2827,18 +2699,14 @@
       <c r="P34" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q34" t="inlineStr"/>
       <c r="R34" t="n">
         <v>0</v>
       </c>
       <c r="S34" t="n">
         <v>0</v>
       </c>
-      <c r="T34" t="n">
-        <v>-0.001</v>
-      </c>
+      <c r="T34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -2897,18 +2765,14 @@
       <c r="P35" t="n">
         <v>0</v>
       </c>
-      <c r="Q35" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q35" t="inlineStr"/>
       <c r="R35" t="n">
         <v>0</v>
       </c>
       <c r="S35" t="n">
         <v>0</v>
       </c>
-      <c r="T35" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -2967,18 +2831,14 @@
       <c r="P36" t="n">
         <v>0</v>
       </c>
-      <c r="Q36" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q36" t="inlineStr"/>
       <c r="R36" t="n">
         <v>0</v>
       </c>
       <c r="S36" t="n">
         <v>0</v>
       </c>
-      <c r="T36" t="n">
-        <v>-0</v>
-      </c>
+      <c r="T36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -3037,18 +2897,14 @@
       <c r="P37" t="n">
         <v>0</v>
       </c>
-      <c r="Q37" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q37" t="inlineStr"/>
       <c r="R37" t="n">
         <v>0</v>
       </c>
       <c r="S37" t="n">
         <v>0</v>
       </c>
-      <c r="T37" t="n">
-        <v>-0.003</v>
-      </c>
+      <c r="T37" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
quick fix of final data value types
</commit_message>
<xml_diff>
--- a/calls_output.xlsx
+++ b/calls_output.xlsx
@@ -551,10 +551,10 @@
         <v>182.25</v>
       </c>
       <c r="F2" t="n">
-        <v>181.87</v>
+        <v>182.01</v>
       </c>
       <c r="G2" t="n">
-        <v>182.12</v>
+        <v>182.26</v>
       </c>
       <c r="H2" t="n">
         <v>0.5299988</v>
@@ -691,10 +691,10 @@
         <v>166.37</v>
       </c>
       <c r="F4" t="n">
-        <v>171.8</v>
+        <v>172.04</v>
       </c>
       <c r="G4" t="n">
-        <v>172.08</v>
+        <v>172.3</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -761,10 +761,10 @@
         <v>169.74</v>
       </c>
       <c r="F5" t="n">
-        <v>166.94</v>
+        <v>167.04</v>
       </c>
       <c r="G5" t="n">
-        <v>167.19</v>
+        <v>167.3</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -831,10 +831,10 @@
         <v>166.53</v>
       </c>
       <c r="F6" t="n">
-        <v>161.77</v>
+        <v>162.11</v>
       </c>
       <c r="G6" t="n">
-        <v>162.11</v>
+        <v>162.38</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -901,10 +901,10 @@
         <v>160.69</v>
       </c>
       <c r="F7" t="n">
-        <v>156.94</v>
+        <v>157.04</v>
       </c>
       <c r="G7" t="n">
-        <v>157.2</v>
+        <v>157.29</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -971,10 +971,10 @@
         <v>156.53</v>
       </c>
       <c r="F8" t="n">
-        <v>151.91</v>
+        <v>152.06</v>
       </c>
       <c r="G8" t="n">
-        <v>152.17</v>
+        <v>152.3</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1111,10 +1111,10 @@
         <v>127.3</v>
       </c>
       <c r="F10" t="n">
-        <v>141.87</v>
+        <v>142.15</v>
       </c>
       <c r="G10" t="n">
-        <v>142.15</v>
+        <v>142.38</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1181,10 +1181,10 @@
         <v>134.86</v>
       </c>
       <c r="F11" t="n">
-        <v>136.92</v>
+        <v>137.07</v>
       </c>
       <c r="G11" t="n">
-        <v>137.18</v>
+        <v>137.31</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1251,10 +1251,10 @@
         <v>129.25</v>
       </c>
       <c r="F12" t="n">
-        <v>131.91</v>
+        <v>132.07</v>
       </c>
       <c r="G12" t="n">
-        <v>132.13</v>
+        <v>132.3</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1321,10 +1321,10 @@
         <v>121.41</v>
       </c>
       <c r="F13" t="n">
-        <v>126.94</v>
+        <v>127.1</v>
       </c>
       <c r="G13" t="n">
-        <v>127.13</v>
+        <v>127.38</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1391,10 +1391,10 @@
         <v>122.01</v>
       </c>
       <c r="F14" t="n">
-        <v>121.9</v>
+        <v>122.08</v>
       </c>
       <c r="G14" t="n">
-        <v>122.15</v>
+        <v>122.32</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1461,10 +1461,10 @@
         <v>114.84</v>
       </c>
       <c r="F15" t="n">
-        <v>116.95</v>
+        <v>117.08</v>
       </c>
       <c r="G15" t="n">
-        <v>117.24</v>
+        <v>117.31</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1531,10 +1531,10 @@
         <v>111.8</v>
       </c>
       <c r="F16" t="n">
-        <v>111.85</v>
+        <v>112.15</v>
       </c>
       <c r="G16" t="n">
-        <v>112.12</v>
+        <v>112.41</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1601,10 +1601,10 @@
         <v>103.11</v>
       </c>
       <c r="F17" t="n">
-        <v>106.93</v>
+        <v>107.16</v>
       </c>
       <c r="G17" t="n">
-        <v>107.17</v>
+        <v>107.37</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1671,10 +1671,10 @@
         <v>99.83</v>
       </c>
       <c r="F18" t="n">
-        <v>101.96</v>
+        <v>102.09</v>
       </c>
       <c r="G18" t="n">
-        <v>102.26</v>
+        <v>102.33</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1741,10 +1741,10 @@
         <v>100.75</v>
       </c>
       <c r="F19" t="n">
-        <v>99.86</v>
+        <v>100.16</v>
       </c>
       <c r="G19" t="n">
-        <v>100.12</v>
+        <v>100.38</v>
       </c>
       <c r="H19" t="n">
         <v>4.5699997</v>
@@ -1811,10 +1811,10 @@
         <v>95.20999999999999</v>
       </c>
       <c r="F20" t="n">
-        <v>98.86</v>
+        <v>99.16</v>
       </c>
       <c r="G20" t="n">
-        <v>99.09999999999999</v>
+        <v>99.42</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -1881,10 +1881,10 @@
         <v>98.77</v>
       </c>
       <c r="F21" t="n">
-        <v>97.93000000000001</v>
+        <v>98.11</v>
       </c>
       <c r="G21" t="n">
-        <v>98.16</v>
+        <v>98.39</v>
       </c>
       <c r="H21" t="n">
         <v>14.119995</v>
@@ -1951,10 +1951,10 @@
         <v>96.63</v>
       </c>
       <c r="F22" t="n">
-        <v>96.93000000000001</v>
+        <v>97.11</v>
       </c>
       <c r="G22" t="n">
-        <v>97.17</v>
+        <v>97.39</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -2299,10 +2299,10 @@
         <v>97.31999999999999</v>
       </c>
       <c r="F27" t="n">
-        <v>92</v>
+        <v>92.17</v>
       </c>
       <c r="G27" t="n">
-        <v>92.27</v>
+        <v>92.38</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -2577,10 +2577,10 @@
         <v>93.37</v>
       </c>
       <c r="F31" t="n">
-        <v>87.97</v>
+        <v>88.13</v>
       </c>
       <c r="G31" t="n">
-        <v>88.18000000000001</v>
+        <v>88.34999999999999</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -2647,10 +2647,10 @@
         <v>87.59</v>
       </c>
       <c r="F32" t="n">
-        <v>86.95999999999999</v>
+        <v>87.09</v>
       </c>
       <c r="G32" t="n">
-        <v>87.22</v>
+        <v>87.34999999999999</v>
       </c>
       <c r="H32" t="n">
         <v>1.6299973</v>
@@ -2717,10 +2717,10 @@
         <v>79.75</v>
       </c>
       <c r="F33" t="n">
-        <v>85.87</v>
+        <v>86.17</v>
       </c>
       <c r="G33" t="n">
-        <v>86.11</v>
+        <v>86.39</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -2787,10 +2787,10 @@
         <v>90.48999999999999</v>
       </c>
       <c r="F34" t="n">
-        <v>84.87</v>
+        <v>85.17</v>
       </c>
       <c r="G34" t="n">
-        <v>85.13</v>
+        <v>85.43000000000001</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -2857,10 +2857,10 @@
         <v>75.52</v>
       </c>
       <c r="F35" t="n">
-        <v>83.95999999999999</v>
+        <v>84.12</v>
       </c>
       <c r="G35" t="n">
-        <v>84.22</v>
+        <v>84.40000000000001</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
@@ -2945,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="L36" t="n">
-        <v>2.227787633666991</v>
+        <v>2.199711531982421</v>
       </c>
       <c r="M36" t="b">
         <v>1</v>
@@ -2961,19 +2961,19 @@
         </is>
       </c>
       <c r="P36" t="n">
-        <v>0.97</v>
+        <v>0.971</v>
       </c>
       <c r="Q36" t="n">
         <v>0.001</v>
       </c>
       <c r="R36" t="n">
-        <v>0.016</v>
+        <v>0.015</v>
       </c>
       <c r="S36" t="n">
         <v>0.008999999999999999</v>
       </c>
       <c r="T36" t="n">
-        <v>-1.807</v>
+        <v>-1.706</v>
       </c>
     </row>
     <row r="37">
@@ -2997,10 +2997,10 @@
         <v>88.51000000000001</v>
       </c>
       <c r="F37" t="n">
-        <v>81.97</v>
+        <v>82.11</v>
       </c>
       <c r="G37" t="n">
-        <v>82.22</v>
+        <v>82.34999999999999</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -3067,10 +3067,10 @@
         <v>81.72</v>
       </c>
       <c r="F38" t="n">
-        <v>80.97</v>
+        <v>81.11</v>
       </c>
       <c r="G38" t="n">
-        <v>81.22</v>
+        <v>81.34999999999999</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -3207,10 +3207,10 @@
         <v>64.67</v>
       </c>
       <c r="F40" t="n">
-        <v>79.01000000000001</v>
+        <v>79.18000000000001</v>
       </c>
       <c r="G40" t="n">
-        <v>79.27</v>
+        <v>79.39</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -3347,10 +3347,10 @@
         <v>75.97</v>
       </c>
       <c r="F42" t="n">
-        <v>76.98</v>
+        <v>77.09999999999999</v>
       </c>
       <c r="G42" t="n">
-        <v>77.27</v>
+        <v>77.34</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -3627,10 +3627,10 @@
         <v>78.45999999999999</v>
       </c>
       <c r="F46" t="n">
-        <v>72.97</v>
+        <v>73.09999999999999</v>
       </c>
       <c r="G46" t="n">
-        <v>73.23</v>
+        <v>73.34</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -3697,10 +3697,10 @@
         <v>67.95999999999999</v>
       </c>
       <c r="F47" t="n">
-        <v>71.94</v>
+        <v>72.09999999999999</v>
       </c>
       <c r="G47" t="n">
-        <v>72.18000000000001</v>
+        <v>72.34</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -3767,10 +3767,10 @@
         <v>71.03</v>
       </c>
       <c r="F48" t="n">
-        <v>70.95</v>
+        <v>71.13</v>
       </c>
       <c r="G48" t="n">
-        <v>71.18000000000001</v>
+        <v>71.41</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -3855,7 +3855,7 @@
         <v>13</v>
       </c>
       <c r="L49" t="n">
-        <v>1.08984830078125</v>
+        <v>0.8281267187499999</v>
       </c>
       <c r="M49" t="b">
         <v>1</v>
@@ -3871,19 +3871,19 @@
         </is>
       </c>
       <c r="P49" t="n">
-        <v>0.999</v>
+        <v>1</v>
       </c>
       <c r="Q49" t="n">
         <v>0</v>
       </c>
       <c r="R49" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="S49" t="n">
         <v>0.01</v>
       </c>
       <c r="T49" t="n">
-        <v>-0.093</v>
+        <v>-0.054</v>
       </c>
     </row>
     <row r="50">
@@ -3907,10 +3907,10 @@
         <v>68.55</v>
       </c>
       <c r="F50" t="n">
-        <v>68.98</v>
+        <v>69.11</v>
       </c>
       <c r="G50" t="n">
-        <v>69.23</v>
+        <v>69.34</v>
       </c>
       <c r="H50" t="n">
         <v>0</v>
@@ -3977,10 +3977,10 @@
         <v>73.09</v>
       </c>
       <c r="F51" t="n">
-        <v>67.95</v>
+        <v>68.11</v>
       </c>
       <c r="G51" t="n">
-        <v>68.19</v>
+        <v>68.37</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -4047,10 +4047,10 @@
         <v>65.95999999999999</v>
       </c>
       <c r="F52" t="n">
-        <v>66.93000000000001</v>
+        <v>67.11</v>
       </c>
       <c r="G52" t="n">
-        <v>67.17</v>
+        <v>67.36</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -4117,10 +4117,10 @@
         <v>72.03</v>
       </c>
       <c r="F53" t="n">
-        <v>66.02</v>
+        <v>66.19</v>
       </c>
       <c r="G53" t="n">
-        <v>66.23</v>
+        <v>66.40000000000001</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -4257,10 +4257,10 @@
         <v>63.18</v>
       </c>
       <c r="F55" t="n">
-        <v>63.99</v>
+        <v>64.11</v>
       </c>
       <c r="G55" t="n">
-        <v>64.28</v>
+        <v>64.34999999999999</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -4327,10 +4327,10 @@
         <v>49.11</v>
       </c>
       <c r="F56" t="n">
-        <v>62.99</v>
+        <v>63.13</v>
       </c>
       <c r="G56" t="n">
-        <v>63.28</v>
+        <v>63.35</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -4397,10 +4397,10 @@
         <v>68.31</v>
       </c>
       <c r="F57" t="n">
-        <v>61.94</v>
+        <v>62.11</v>
       </c>
       <c r="G57" t="n">
-        <v>62.19</v>
+        <v>62.37</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -4467,10 +4467,10 @@
         <v>60.19</v>
       </c>
       <c r="F58" t="n">
-        <v>60.94</v>
+        <v>61.13</v>
       </c>
       <c r="G58" t="n">
-        <v>61.19</v>
+        <v>61.36</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -4537,10 +4537,10 @@
         <v>59.51</v>
       </c>
       <c r="F59" t="n">
-        <v>59.94</v>
+        <v>60.11</v>
       </c>
       <c r="G59" t="n">
-        <v>60.19</v>
+        <v>60.35</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -4607,10 +4607,10 @@
         <v>58.56</v>
       </c>
       <c r="F60" t="n">
-        <v>58.95</v>
+        <v>59.12</v>
       </c>
       <c r="G60" t="n">
-        <v>59.19</v>
+        <v>59.35</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -4677,10 +4677,10 @@
         <v>57.86</v>
       </c>
       <c r="F61" t="n">
-        <v>57.88</v>
+        <v>58.1</v>
       </c>
       <c r="G61" t="n">
-        <v>58.16</v>
+        <v>58.34</v>
       </c>
       <c r="H61" t="n">
         <v>0.3199997</v>
@@ -4747,10 +4747,10 @@
         <v>57.38</v>
       </c>
       <c r="F62" t="n">
-        <v>56.89</v>
+        <v>57.16</v>
       </c>
       <c r="G62" t="n">
-        <v>57.13</v>
+        <v>57.46</v>
       </c>
       <c r="H62" t="n">
         <v>1.5400009</v>
@@ -4817,10 +4817,10 @@
         <v>49.22</v>
       </c>
       <c r="F63" t="n">
-        <v>55.9</v>
+        <v>56.16</v>
       </c>
       <c r="G63" t="n">
-        <v>56.16</v>
+        <v>56.39</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -4887,10 +4887,10 @@
         <v>58.71</v>
       </c>
       <c r="F64" t="n">
-        <v>54.97</v>
+        <v>55.13</v>
       </c>
       <c r="G64" t="n">
-        <v>55.18</v>
+        <v>55.38</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -4957,10 +4957,10 @@
         <v>59.92</v>
       </c>
       <c r="F65" t="n">
-        <v>53.96</v>
+        <v>54.2</v>
       </c>
       <c r="G65" t="n">
-        <v>54.21</v>
+        <v>54.41</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -5027,10 +5027,10 @@
         <v>58.15</v>
       </c>
       <c r="F66" t="n">
-        <v>53.03</v>
+        <v>53.2</v>
       </c>
       <c r="G66" t="n">
-        <v>53.29</v>
+        <v>53.41</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -5097,10 +5097,10 @@
         <v>51.46</v>
       </c>
       <c r="F67" t="n">
-        <v>51.94</v>
+        <v>52.14</v>
       </c>
       <c r="G67" t="n">
-        <v>52.19</v>
+        <v>52.36</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -5167,10 +5167,10 @@
         <v>50.32</v>
       </c>
       <c r="F68" t="n">
-        <v>51</v>
+        <v>51.14</v>
       </c>
       <c r="G68" t="n">
-        <v>51.29</v>
+        <v>51.37</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -5237,10 +5237,10 @@
         <v>49.56</v>
       </c>
       <c r="F69" t="n">
-        <v>49.9</v>
+        <v>50.23</v>
       </c>
       <c r="G69" t="n">
-        <v>50.16</v>
+        <v>50.48</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -5307,10 +5307,10 @@
         <v>54.01</v>
       </c>
       <c r="F70" t="n">
-        <v>48.99</v>
+        <v>49.12</v>
       </c>
       <c r="G70" t="n">
-        <v>49.25</v>
+        <v>49.36</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -5377,10 +5377,10 @@
         <v>46.92</v>
       </c>
       <c r="F71" t="n">
-        <v>47.96</v>
+        <v>48.13</v>
       </c>
       <c r="G71" t="n">
-        <v>48.2</v>
+        <v>48.36</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -5447,10 +5447,10 @@
         <v>46.01</v>
       </c>
       <c r="F72" t="n">
-        <v>46.89</v>
+        <v>47.11</v>
       </c>
       <c r="G72" t="n">
-        <v>47.13</v>
+        <v>47.35</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -5517,10 +5517,10 @@
         <v>44.92</v>
       </c>
       <c r="F73" t="n">
-        <v>45.91</v>
+        <v>46.23</v>
       </c>
       <c r="G73" t="n">
-        <v>46.17</v>
+        <v>46.48</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -5587,10 +5587,10 @@
         <v>50.98</v>
       </c>
       <c r="F74" t="n">
-        <v>44.98</v>
+        <v>45.21</v>
       </c>
       <c r="G74" t="n">
-        <v>45.3</v>
+        <v>45.4</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -5657,10 +5657,10 @@
         <v>47.66</v>
       </c>
       <c r="F75" t="n">
-        <v>44.01</v>
+        <v>44.13</v>
       </c>
       <c r="G75" t="n">
-        <v>44.26</v>
+        <v>44.39</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -5727,10 +5727,10 @@
         <v>42.08</v>
       </c>
       <c r="F76" t="n">
-        <v>42.86</v>
+        <v>43.14</v>
       </c>
       <c r="G76" t="n">
-        <v>43.16</v>
+        <v>43.37</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -5797,10 +5797,10 @@
         <v>41.89</v>
       </c>
       <c r="F77" t="n">
-        <v>41.9</v>
+        <v>42.16</v>
       </c>
       <c r="G77" t="n">
-        <v>42.21</v>
+        <v>42.37</v>
       </c>
       <c r="H77" t="n">
         <v>3.8999977</v>
@@ -5867,10 +5867,10 @@
         <v>44.4</v>
       </c>
       <c r="F78" t="n">
-        <v>41</v>
+        <v>41.15</v>
       </c>
       <c r="G78" t="n">
-        <v>41.26</v>
+        <v>41.37</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -5937,10 +5937,10 @@
         <v>38.75</v>
       </c>
       <c r="F79" t="n">
-        <v>39.98</v>
+        <v>40.15</v>
       </c>
       <c r="G79" t="n">
-        <v>40.22</v>
+        <v>40.38</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -6007,10 +6007,10 @@
         <v>37.95</v>
       </c>
       <c r="F80" t="n">
-        <v>39</v>
+        <v>39.13</v>
       </c>
       <c r="G80" t="n">
-        <v>39.26</v>
+        <v>39.37</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -6077,10 +6077,10 @@
         <v>37.36</v>
       </c>
       <c r="F81" t="n">
-        <v>37.97</v>
+        <v>38.14</v>
       </c>
       <c r="G81" t="n">
-        <v>38.21</v>
+        <v>38.37</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -6147,10 +6147,10 @@
         <v>37.43</v>
       </c>
       <c r="F82" t="n">
-        <v>36.99</v>
+        <v>37.15</v>
       </c>
       <c r="G82" t="n">
-        <v>37.2</v>
+        <v>37.4</v>
       </c>
       <c r="H82" t="n">
         <v>1.0999985</v>
@@ -6217,10 +6217,10 @@
         <v>34.54</v>
       </c>
       <c r="F83" t="n">
-        <v>35.98</v>
+        <v>36.15</v>
       </c>
       <c r="G83" t="n">
-        <v>36.21</v>
+        <v>36.39</v>
       </c>
       <c r="H83" t="n">
         <v>0</v>
@@ -6287,10 +6287,10 @@
         <v>34.82</v>
       </c>
       <c r="F84" t="n">
-        <v>34.77</v>
+        <v>35.18</v>
       </c>
       <c r="G84" t="n">
-        <v>35.15</v>
+        <v>35.41</v>
       </c>
       <c r="H84" t="n">
         <v>4.029999</v>
@@ -6357,10 +6357,10 @@
         <v>31.88</v>
       </c>
       <c r="F85" t="n">
-        <v>33.98</v>
+        <v>34.22</v>
       </c>
       <c r="G85" t="n">
-        <v>34.23</v>
+        <v>34.43</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -6427,10 +6427,10 @@
         <v>29.31</v>
       </c>
       <c r="F86" t="n">
-        <v>33</v>
+        <v>33.22</v>
       </c>
       <c r="G86" t="n">
-        <v>33.23</v>
+        <v>33.43</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -6497,10 +6497,10 @@
         <v>28.54</v>
       </c>
       <c r="F87" t="n">
-        <v>32.02</v>
+        <v>32.16</v>
       </c>
       <c r="G87" t="n">
-        <v>32.23</v>
+        <v>32.43</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -6567,10 +6567,10 @@
         <v>30.88</v>
       </c>
       <c r="F88" t="n">
-        <v>30.9</v>
+        <v>31.17</v>
       </c>
       <c r="G88" t="n">
-        <v>31.14</v>
+        <v>31.38</v>
       </c>
       <c r="H88" t="n">
         <v>1.3799992</v>
@@ -6637,10 +6637,10 @@
         <v>28.72</v>
       </c>
       <c r="F89" t="n">
-        <v>30.01</v>
+        <v>30.14</v>
       </c>
       <c r="G89" t="n">
-        <v>30.27</v>
+        <v>30.38</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -6707,10 +6707,10 @@
         <v>27.86</v>
       </c>
       <c r="F90" t="n">
-        <v>28.92</v>
+        <v>29.18</v>
       </c>
       <c r="G90" t="n">
-        <v>29.16</v>
+        <v>29.48</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -6777,10 +6777,10 @@
         <v>27.24</v>
       </c>
       <c r="F91" t="n">
-        <v>27.91</v>
+        <v>28.13</v>
       </c>
       <c r="G91" t="n">
-        <v>28.19</v>
+        <v>28.37</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -6847,10 +6847,10 @@
         <v>27.44</v>
       </c>
       <c r="F92" t="n">
-        <v>26.99</v>
+        <v>27.19</v>
       </c>
       <c r="G92" t="n">
-        <v>27.32</v>
+        <v>27.42</v>
       </c>
       <c r="H92" t="n">
         <v>0.32999992</v>
@@ -6917,10 +6917,10 @@
         <v>26.83</v>
       </c>
       <c r="F93" t="n">
-        <v>25.89</v>
+        <v>26.23</v>
       </c>
       <c r="G93" t="n">
-        <v>26.24</v>
+        <v>26.49</v>
       </c>
       <c r="H93" t="n">
         <v>1.2700005</v>
@@ -6987,10 +6987,10 @@
         <v>25.82</v>
       </c>
       <c r="F94" t="n">
-        <v>24.99</v>
+        <v>25.23</v>
       </c>
       <c r="G94" t="n">
-        <v>25.24</v>
+        <v>25.44</v>
       </c>
       <c r="H94" t="n">
         <v>2.0900002</v>
@@ -7057,10 +7057,10 @@
         <v>24.91</v>
       </c>
       <c r="F95" t="n">
-        <v>24.03</v>
+        <v>24.17</v>
       </c>
       <c r="G95" t="n">
-        <v>24.24</v>
+        <v>24.44</v>
       </c>
       <c r="H95" t="n">
         <v>1.7600002</v>
@@ -7127,10 +7127,10 @@
         <v>22.63</v>
       </c>
       <c r="F96" t="n">
-        <v>22.93</v>
+        <v>23.26</v>
       </c>
       <c r="G96" t="n">
-        <v>23.19</v>
+        <v>23.5</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -7194,22 +7194,22 @@
         <v>415</v>
       </c>
       <c r="E97" t="n">
-        <v>22.13</v>
+        <v>22.4</v>
       </c>
       <c r="F97" t="n">
-        <v>21.99</v>
+        <v>22.25</v>
       </c>
       <c r="G97" t="n">
-        <v>22.23</v>
+        <v>22.48</v>
       </c>
       <c r="H97" t="n">
-        <v>0.15999985</v>
+        <v>0.4300003</v>
       </c>
       <c r="I97" t="n">
-        <v>0.72826517</v>
+        <v>1.9572158</v>
       </c>
       <c r="J97" t="n">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="K97" t="n">
         <v>568</v>
@@ -7267,10 +7267,10 @@
         <v>21.15</v>
       </c>
       <c r="F98" t="n">
-        <v>21.03</v>
+        <v>21.23</v>
       </c>
       <c r="G98" t="n">
-        <v>21.28</v>
+        <v>21.46</v>
       </c>
       <c r="H98" t="n">
         <v>2.959999</v>
@@ -7337,10 +7337,10 @@
         <v>19.15</v>
       </c>
       <c r="F99" t="n">
-        <v>20.03</v>
+        <v>20.17</v>
       </c>
       <c r="G99" t="n">
-        <v>20.28</v>
+        <v>20.41</v>
       </c>
       <c r="H99" t="n">
         <v>1.1399994</v>
@@ -7407,10 +7407,10 @@
         <v>17.95</v>
       </c>
       <c r="F100" t="n">
-        <v>19</v>
+        <v>19.17</v>
       </c>
       <c r="G100" t="n">
-        <v>19.25</v>
+        <v>19.39</v>
       </c>
       <c r="H100" t="n">
         <v>0</v>
@@ -7477,10 +7477,10 @@
         <v>14.74</v>
       </c>
       <c r="F101" t="n">
-        <v>18.03</v>
+        <v>18.18</v>
       </c>
       <c r="G101" t="n">
-        <v>18.27</v>
+        <v>18.45</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
@@ -7547,10 +7547,10 @@
         <v>17.57</v>
       </c>
       <c r="F102" t="n">
-        <v>17.03</v>
+        <v>17.14</v>
       </c>
       <c r="G102" t="n">
-        <v>17.29</v>
+        <v>17.37</v>
       </c>
       <c r="H102" t="n">
         <v>1.7599993</v>
@@ -7617,10 +7617,10 @@
         <v>17.3</v>
       </c>
       <c r="F103" t="n">
-        <v>15.93</v>
+        <v>16.24</v>
       </c>
       <c r="G103" t="n">
-        <v>16.18</v>
+        <v>16.5</v>
       </c>
       <c r="H103" t="n">
         <v>2.8099995</v>
@@ -7687,10 +7687,10 @@
         <v>14.82</v>
       </c>
       <c r="F104" t="n">
-        <v>15.01</v>
+        <v>15.17</v>
       </c>
       <c r="G104" t="n">
-        <v>15.26</v>
+        <v>15.43</v>
       </c>
       <c r="H104" t="n">
         <v>0.5799999</v>
@@ -7757,10 +7757,10 @@
         <v>14.84</v>
       </c>
       <c r="F105" t="n">
-        <v>13.94</v>
+        <v>14.2</v>
       </c>
       <c r="G105" t="n">
-        <v>14.18</v>
+        <v>14.44</v>
       </c>
       <c r="H105" t="n">
         <v>0.8400001499999999</v>
@@ -7827,10 +7827,10 @@
         <v>13.2</v>
       </c>
       <c r="F106" t="n">
-        <v>13.08</v>
+        <v>13.21</v>
       </c>
       <c r="G106" t="n">
-        <v>13.35</v>
+        <v>13.46</v>
       </c>
       <c r="H106" t="n">
         <v>1.3199997</v>
@@ -7897,10 +7897,10 @@
         <v>12.29</v>
       </c>
       <c r="F107" t="n">
-        <v>11.92</v>
+        <v>12.17</v>
       </c>
       <c r="G107" t="n">
-        <v>12.19</v>
+        <v>12.46</v>
       </c>
       <c r="H107" t="n">
         <v>1.4399996</v>
@@ -7967,10 +7967,10 @@
         <v>11.36</v>
       </c>
       <c r="F108" t="n">
-        <v>11.01</v>
+        <v>11.2</v>
       </c>
       <c r="G108" t="n">
-        <v>11.25</v>
+        <v>11.44</v>
       </c>
       <c r="H108" t="n">
         <v>1.1899996</v>
@@ -8037,10 +8037,10 @@
         <v>10.11</v>
       </c>
       <c r="F109" t="n">
-        <v>10.1</v>
+        <v>10.21</v>
       </c>
       <c r="G109" t="n">
-        <v>10.25</v>
+        <v>10.4</v>
       </c>
       <c r="H109" t="n">
         <v>0.069999695</v>
@@ -8107,10 +8107,10 @@
         <v>9.300000000000001</v>
       </c>
       <c r="F110" t="n">
-        <v>9.039999999999999</v>
+        <v>9.19</v>
       </c>
       <c r="G110" t="n">
-        <v>9.279999999999999</v>
+        <v>9.43</v>
       </c>
       <c r="H110" t="n">
         <v>0.6500006</v>
@@ -8174,22 +8174,22 @@
         <v>429</v>
       </c>
       <c r="E111" t="n">
-        <v>8.15</v>
+        <v>8.34</v>
       </c>
       <c r="F111" t="n">
-        <v>8.050000000000001</v>
+        <v>8.23</v>
       </c>
       <c r="G111" t="n">
-        <v>8.289999999999999</v>
+        <v>8.44</v>
       </c>
       <c r="H111" t="n">
-        <v>0.14999962</v>
+        <v>0.34000015</v>
       </c>
       <c r="I111" t="n">
-        <v>1.8749952</v>
+        <v>4.250002</v>
       </c>
       <c r="J111" t="n">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="K111" t="n">
         <v>2052</v>
@@ -8244,28 +8244,28 @@
         <v>430</v>
       </c>
       <c r="E112" t="n">
-        <v>7.22</v>
+        <v>7.35</v>
       </c>
       <c r="F112" t="n">
-        <v>7.13</v>
+        <v>7.23</v>
       </c>
       <c r="G112" t="n">
-        <v>7.37</v>
+        <v>7.49</v>
       </c>
       <c r="H112" t="n">
-        <v>0.21999979</v>
+        <v>0.3499999</v>
       </c>
       <c r="I112" t="n">
-        <v>3.1428542</v>
+        <v>4.999999</v>
       </c>
       <c r="J112" t="n">
-        <v>2602</v>
+        <v>2622</v>
       </c>
       <c r="K112" t="n">
         <v>30216</v>
       </c>
       <c r="L112" t="n">
-        <v>0.09766527343750001</v>
+        <v>1e-05</v>
       </c>
       <c r="M112" t="b">
         <v>1</v>
@@ -8284,7 +8284,7 @@
         <v>1</v>
       </c>
       <c r="Q112" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="R112" t="n">
         <v>0</v>
@@ -8293,7 +8293,7 @@
         <v>0.012</v>
       </c>
       <c r="T112" t="n">
-        <v>-0.063</v>
+        <v>-0.062</v>
       </c>
     </row>
     <row r="113">
@@ -8314,22 +8314,22 @@
         <v>431</v>
       </c>
       <c r="E113" t="n">
-        <v>6.42</v>
+        <v>6.34</v>
       </c>
       <c r="F113" t="n">
-        <v>6.08</v>
+        <v>6.32</v>
       </c>
       <c r="G113" t="n">
-        <v>6.28</v>
+        <v>6.49</v>
       </c>
       <c r="H113" t="n">
-        <v>0.28999996</v>
+        <v>0.21000004</v>
       </c>
       <c r="I113" t="n">
-        <v>4.730831</v>
+        <v>3.4257755</v>
       </c>
       <c r="J113" t="n">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="K113" t="n">
         <v>2101</v>
@@ -8384,28 +8384,28 @@
         <v>432</v>
       </c>
       <c r="E114" t="n">
-        <v>5.18</v>
+        <v>5.5</v>
       </c>
       <c r="F114" t="n">
-        <v>5.16</v>
+        <v>5.37</v>
       </c>
       <c r="G114" t="n">
-        <v>5.37</v>
+        <v>5.55</v>
       </c>
       <c r="H114" t="n">
-        <v>-0.059999943</v>
+        <v>0.26000023</v>
       </c>
       <c r="I114" t="n">
-        <v>-1.1450372</v>
+        <v>4.961837</v>
       </c>
       <c r="J114" t="n">
-        <v>977</v>
+        <v>1026</v>
       </c>
       <c r="K114" t="n">
         <v>6856</v>
       </c>
       <c r="L114" t="n">
-        <v>0.07422800781250001</v>
+        <v>0.09180595703125</v>
       </c>
       <c r="M114" t="b">
         <v>1</v>
@@ -8421,19 +8421,19 @@
         </is>
       </c>
       <c r="P114" t="n">
-        <v>0.999</v>
+        <v>0.996</v>
       </c>
       <c r="Q114" t="n">
-        <v>0.001</v>
+        <v>0.005</v>
       </c>
       <c r="R114" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="S114" t="n">
         <v>0.012</v>
       </c>
       <c r="T114" t="n">
-        <v>-0.064</v>
+        <v>-0.074</v>
       </c>
     </row>
     <row r="115">
@@ -8454,28 +8454,28 @@
         <v>433</v>
       </c>
       <c r="E115" t="n">
-        <v>4.31</v>
+        <v>4.5</v>
       </c>
       <c r="F115" t="n">
-        <v>4.25</v>
+        <v>4.38</v>
       </c>
       <c r="G115" t="n">
-        <v>4.43</v>
+        <v>4.54</v>
       </c>
       <c r="H115" t="n">
-        <v>-0.07000017</v>
+        <v>0.119999886</v>
       </c>
       <c r="I115" t="n">
-        <v>-1.5981774</v>
+        <v>2.7397234</v>
       </c>
       <c r="J115" t="n">
-        <v>1472</v>
+        <v>1490</v>
       </c>
       <c r="K115" t="n">
         <v>13287</v>
       </c>
       <c r="L115" t="n">
-        <v>0.08643491699218751</v>
+        <v>0.073251455078125</v>
       </c>
       <c r="M115" t="b">
         <v>1</v>
@@ -8491,19 +8491,19 @@
         </is>
       </c>
       <c r="P115" t="n">
-        <v>0.988</v>
+        <v>0.997</v>
       </c>
       <c r="Q115" t="n">
-        <v>0.015</v>
+        <v>0.005</v>
       </c>
       <c r="R115" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="S115" t="n">
         <v>0.012</v>
       </c>
       <c r="T115" t="n">
-        <v>-0.092</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="116">
@@ -8524,28 +8524,28 @@
         <v>434</v>
       </c>
       <c r="E116" t="n">
-        <v>3.43</v>
+        <v>3.62</v>
       </c>
       <c r="F116" t="n">
-        <v>3.42</v>
+        <v>3.53</v>
       </c>
       <c r="G116" t="n">
-        <v>3.45</v>
+        <v>3.67</v>
       </c>
       <c r="H116" t="n">
-        <v>-0.20000005</v>
+        <v>-0.010000229</v>
       </c>
       <c r="I116" t="n">
-        <v>-5.5096426</v>
+        <v>-0.27548838</v>
       </c>
       <c r="J116" t="n">
-        <v>4640</v>
+        <v>4671</v>
       </c>
       <c r="K116" t="n">
         <v>19106</v>
       </c>
       <c r="L116" t="n">
-        <v>0.07471628417968751</v>
+        <v>0.0893645751953125</v>
       </c>
       <c r="M116" t="b">
         <v>1</v>
@@ -8561,19 +8561,19 @@
         </is>
       </c>
       <c r="P116" t="n">
-        <v>0.979</v>
+        <v>0.961</v>
       </c>
       <c r="Q116" t="n">
-        <v>0.029</v>
+        <v>0.041</v>
       </c>
       <c r="R116" t="n">
-        <v>0.012</v>
+        <v>0.019</v>
       </c>
       <c r="S116" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T116" t="n">
-        <v>-0.104</v>
+        <v>-0.147</v>
       </c>
     </row>
     <row r="117">
@@ -8594,28 +8594,28 @@
         <v>435</v>
       </c>
       <c r="E117" t="n">
-        <v>2.69</v>
+        <v>2.77</v>
       </c>
       <c r="F117" t="n">
-        <v>2.61</v>
+        <v>2.8</v>
       </c>
       <c r="G117" t="n">
-        <v>2.69</v>
+        <v>2.82</v>
       </c>
       <c r="H117" t="n">
-        <v>-0.23000002</v>
+        <v>-0.1500001</v>
       </c>
       <c r="I117" t="n">
-        <v>-7.876713</v>
+        <v>-5.1369896</v>
       </c>
       <c r="J117" t="n">
-        <v>29617</v>
+        <v>30143</v>
       </c>
       <c r="K117" t="n">
         <v>30201</v>
       </c>
       <c r="L117" t="n">
-        <v>0.08863216064453125</v>
+        <v>0.0893645751953125</v>
       </c>
       <c r="M117" t="b">
         <v>1</v>
@@ -8631,19 +8631,19 @@
         </is>
       </c>
       <c r="P117" t="n">
-        <v>0.889</v>
+        <v>0.898</v>
       </c>
       <c r="Q117" t="n">
-        <v>0.093</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="R117" t="n">
-        <v>0.043</v>
+        <v>0.041</v>
       </c>
       <c r="S117" t="n">
         <v>0.011</v>
       </c>
       <c r="T117" t="n">
-        <v>-0.248</v>
+        <v>-0.239</v>
       </c>
     </row>
     <row r="118">
@@ -8664,28 +8664,28 @@
         <v>436</v>
       </c>
       <c r="E118" t="n">
-        <v>2.05</v>
+        <v>2.14</v>
       </c>
       <c r="F118" t="n">
-        <v>1.99</v>
+        <v>2.1</v>
       </c>
       <c r="G118" t="n">
-        <v>2</v>
+        <v>2.11</v>
       </c>
       <c r="H118" t="n">
-        <v>-0.21000004</v>
+        <v>-0.119999886</v>
       </c>
       <c r="I118" t="n">
-        <v>-9.292037000000001</v>
+        <v>-5.3097296</v>
       </c>
       <c r="J118" t="n">
-        <v>64505</v>
+        <v>66970</v>
       </c>
       <c r="K118" t="n">
         <v>18735</v>
       </c>
       <c r="L118" t="n">
-        <v>0.09302664794921875</v>
+        <v>0.09327078613281251</v>
       </c>
       <c r="M118" t="b">
         <v>1</v>
@@ -8701,19 +8701,19 @@
         </is>
       </c>
       <c r="P118" t="n">
-        <v>0.755</v>
+        <v>0.772</v>
       </c>
       <c r="Q118" t="n">
-        <v>0.148</v>
+        <v>0.142</v>
       </c>
       <c r="R118" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="S118" t="n">
         <v>0.008999999999999999</v>
       </c>
       <c r="T118" t="n">
-        <v>-0.382</v>
+        <v>-0.371</v>
       </c>
     </row>
     <row r="119">
@@ -8734,28 +8734,28 @@
         <v>437</v>
       </c>
       <c r="E119" t="n">
-        <v>1.44</v>
+        <v>1.54</v>
       </c>
       <c r="F119" t="n">
-        <v>1.45</v>
+        <v>1.48</v>
       </c>
       <c r="G119" t="n">
-        <v>1.46</v>
+        <v>1.49</v>
       </c>
       <c r="H119" t="n">
-        <v>-0.25</v>
+        <v>-0.1500001</v>
       </c>
       <c r="I119" t="n">
-        <v>-14.792898</v>
+        <v>-8.875745</v>
       </c>
       <c r="J119" t="n">
-        <v>140362</v>
+        <v>143392</v>
       </c>
       <c r="K119" t="n">
         <v>17089</v>
       </c>
       <c r="L119" t="n">
-        <v>0.09851975708007812</v>
+        <v>0.09412526977539062</v>
       </c>
       <c r="M119" t="b">
         <v>1</v>
@@ -8771,19 +8771,19 @@
         </is>
       </c>
       <c r="P119" t="n">
-        <v>0.582</v>
+        <v>0.608</v>
       </c>
       <c r="Q119" t="n">
-        <v>0.173</v>
+        <v>0.178</v>
       </c>
       <c r="R119" t="n">
-        <v>0.089</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="S119" t="n">
         <v>0.007</v>
       </c>
       <c r="T119" t="n">
-        <v>-0.477</v>
+        <v>-0.452</v>
       </c>
     </row>
     <row r="120">
@@ -8804,28 +8804,28 @@
         <v>438</v>
       </c>
       <c r="E120" t="n">
-        <v>0.98</v>
+        <v>1.04</v>
       </c>
       <c r="F120" t="n">
-        <v>0.97</v>
+        <v>1.04</v>
       </c>
       <c r="G120" t="n">
-        <v>0.98</v>
+        <v>1.05</v>
       </c>
       <c r="H120" t="n">
-        <v>-0.25</v>
+        <v>-0.19000006</v>
       </c>
       <c r="I120" t="n">
-        <v>-20.325203</v>
+        <v>-15.447159</v>
       </c>
       <c r="J120" t="n">
-        <v>163618</v>
+        <v>167479</v>
       </c>
       <c r="K120" t="n">
         <v>21427</v>
       </c>
       <c r="L120" t="n">
-        <v>0.098641826171875</v>
+        <v>0.09888596435546876</v>
       </c>
       <c r="M120" t="b">
         <v>0</v>
@@ -8841,19 +8841,19 @@
         </is>
       </c>
       <c r="P120" t="n">
-        <v>0.407</v>
+        <v>0.428</v>
       </c>
       <c r="Q120" t="n">
-        <v>0.172</v>
+        <v>0.173</v>
       </c>
       <c r="R120" t="n">
-        <v>0.089</v>
+        <v>0.09</v>
       </c>
       <c r="S120" t="n">
         <v>0.005</v>
       </c>
       <c r="T120" t="n">
-        <v>-0.464</v>
+        <v>-0.471</v>
       </c>
     </row>
     <row r="121">
@@ -8874,28 +8874,28 @@
         <v>439</v>
       </c>
       <c r="E121" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="F121" t="n">
         <v>0.64</v>
       </c>
-      <c r="F121" t="n">
-        <v>0.63</v>
-      </c>
       <c r="G121" t="n">
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
       <c r="H121" t="n">
-        <v>-0.21000004</v>
+        <v>-0.19</v>
       </c>
       <c r="I121" t="n">
-        <v>-24.705887</v>
+        <v>-22.35294</v>
       </c>
       <c r="J121" t="n">
-        <v>70625</v>
+        <v>71417</v>
       </c>
       <c r="K121" t="n">
         <v>16838</v>
       </c>
       <c r="L121" t="n">
-        <v>0.1003507934570312</v>
+        <v>0.09693285888671876</v>
       </c>
       <c r="M121" t="b">
         <v>0</v>
@@ -8911,19 +8911,19 @@
         </is>
       </c>
       <c r="P121" t="n">
-        <v>0.253</v>
+        <v>0.263</v>
       </c>
       <c r="Q121" t="n">
-        <v>0.139</v>
+        <v>0.147</v>
       </c>
       <c r="R121" t="n">
-        <v>0.073</v>
+        <v>0.075</v>
       </c>
       <c r="S121" t="n">
         <v>0.003</v>
       </c>
       <c r="T121" t="n">
-        <v>-0.383</v>
+        <v>-0.379</v>
       </c>
     </row>
     <row r="122">
@@ -8944,28 +8944,28 @@
         <v>440</v>
       </c>
       <c r="E122" t="n">
-        <v>0.4</v>
+        <v>0.42</v>
       </c>
       <c r="F122" t="n">
-        <v>0.39</v>
+        <v>0.41</v>
       </c>
       <c r="G122" t="n">
-        <v>0.4</v>
+        <v>0.42</v>
       </c>
       <c r="H122" t="n">
-        <v>-0.16999999</v>
+        <v>-0.15</v>
       </c>
       <c r="I122" t="n">
-        <v>-29.82456</v>
+        <v>-26.31579</v>
       </c>
       <c r="J122" t="n">
-        <v>85538</v>
+        <v>87395</v>
       </c>
       <c r="K122" t="n">
         <v>38206</v>
       </c>
       <c r="L122" t="n">
-        <v>0.1020597607421875</v>
+        <v>0.100594931640625</v>
       </c>
       <c r="M122" t="b">
         <v>0</v>
@@ -8981,19 +8981,19 @@
         </is>
       </c>
       <c r="P122" t="n">
-        <v>0.14</v>
+        <v>0.148</v>
       </c>
       <c r="Q122" t="n">
-        <v>0.095</v>
+        <v>0.1</v>
       </c>
       <c r="R122" t="n">
-        <v>0.051</v>
+        <v>0.053</v>
       </c>
       <c r="S122" t="n">
         <v>0.002</v>
       </c>
       <c r="T122" t="n">
-        <v>-0.269</v>
+        <v>-0.276</v>
       </c>
     </row>
     <row r="123">
@@ -9014,28 +9014,28 @@
         <v>441</v>
       </c>
       <c r="E123" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F123" t="n">
         <v>0.24</v>
       </c>
-      <c r="F123" t="n">
-        <v>0.22</v>
-      </c>
       <c r="G123" t="n">
-        <v>0.23</v>
+        <v>0.25</v>
       </c>
       <c r="H123" t="n">
-        <v>-0.13000001</v>
+        <v>-0.120000005</v>
       </c>
       <c r="I123" t="n">
-        <v>-35.13514</v>
+        <v>-32.432434</v>
       </c>
       <c r="J123" t="n">
-        <v>29711</v>
+        <v>31504</v>
       </c>
       <c r="K123" t="n">
         <v>13128</v>
       </c>
       <c r="L123" t="n">
-        <v>0.1020597607421875</v>
+        <v>0.1018156225585937</v>
       </c>
       <c r="M123" t="b">
         <v>0</v>
@@ -9051,19 +9051,19 @@
         </is>
       </c>
       <c r="P123" t="n">
-        <v>0.066</v>
+        <v>0.073</v>
       </c>
       <c r="Q123" t="n">
-        <v>0.055</v>
+        <v>0.059</v>
       </c>
       <c r="R123" t="n">
-        <v>0.029</v>
+        <v>0.032</v>
       </c>
       <c r="S123" t="n">
         <v>0.001</v>
       </c>
       <c r="T123" t="n">
-        <v>-0.154</v>
+        <v>-0.165</v>
       </c>
     </row>
     <row r="124">
@@ -9084,28 +9084,28 @@
         <v>442</v>
       </c>
       <c r="E124" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="F124" t="n">
         <v>0.14</v>
       </c>
-      <c r="F124" t="n">
-        <v>0.13</v>
-      </c>
       <c r="G124" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="H124" t="n">
-        <v>-0.08</v>
+        <v>-0.06999999</v>
       </c>
       <c r="I124" t="n">
-        <v>-36.363636</v>
+        <v>-31.818178</v>
       </c>
       <c r="J124" t="n">
-        <v>32111</v>
+        <v>32294</v>
       </c>
       <c r="K124" t="n">
         <v>36827</v>
       </c>
       <c r="L124" t="n">
-        <v>0.1054776953125</v>
+        <v>0.1047452807617187</v>
       </c>
       <c r="M124" t="b">
         <v>0</v>
@@ -9121,19 +9121,19 @@
         </is>
       </c>
       <c r="P124" t="n">
+        <v>0.034</v>
+      </c>
+      <c r="Q124" t="n">
         <v>0.031</v>
       </c>
-      <c r="Q124" t="n">
-        <v>0.029</v>
-      </c>
       <c r="R124" t="n">
-        <v>0.016</v>
+        <v>0.017</v>
       </c>
       <c r="S124" t="n">
         <v>0</v>
       </c>
       <c r="T124" t="n">
-        <v>-0.08599999999999999</v>
+        <v>-0.092</v>
       </c>
     </row>
     <row r="125">
@@ -9169,13 +9169,13 @@
         <v>-42.857143</v>
       </c>
       <c r="J125" t="n">
-        <v>13078</v>
+        <v>13143</v>
       </c>
       <c r="K125" t="n">
         <v>7898</v>
       </c>
       <c r="L125" t="n">
-        <v>0.110360458984375</v>
+        <v>0.1079190771484375</v>
       </c>
       <c r="M125" t="b">
         <v>0</v>
@@ -9203,7 +9203,7 @@
         <v>0</v>
       </c>
       <c r="T125" t="n">
-        <v>-0.048</v>
+        <v>-0.047</v>
       </c>
     </row>
     <row r="126">
@@ -9224,7 +9224,7 @@
         <v>444</v>
       </c>
       <c r="E126" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="F126" t="n">
         <v>0.05</v>
@@ -9233,19 +9233,19 @@
         <v>0.06</v>
       </c>
       <c r="H126" t="n">
-        <v>-0.029999997</v>
+        <v>-0.02</v>
       </c>
       <c r="I126" t="n">
-        <v>-37.499996</v>
+        <v>-25</v>
       </c>
       <c r="J126" t="n">
-        <v>8924</v>
+        <v>9355</v>
       </c>
       <c r="K126" t="n">
         <v>6936</v>
       </c>
       <c r="L126" t="n">
-        <v>0.1157314990234375</v>
+        <v>0.1132901171875</v>
       </c>
       <c r="M126" t="b">
         <v>0</v>
@@ -9273,7 +9273,7 @@
         <v>0</v>
       </c>
       <c r="T126" t="n">
-        <v>-0.027</v>
+        <v>-0.026</v>
       </c>
     </row>
     <row r="127">
@@ -9309,13 +9309,13 @@
         <v>0</v>
       </c>
       <c r="J127" t="n">
-        <v>6837</v>
+        <v>6903</v>
       </c>
       <c r="K127" t="n">
         <v>21998</v>
       </c>
       <c r="L127" t="n">
-        <v>0.1211025390625</v>
+        <v>0.11914943359375</v>
       </c>
       <c r="M127" t="b">
         <v>0</v>
@@ -9364,7 +9364,7 @@
         <v>446</v>
       </c>
       <c r="E128" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F128" t="n">
         <v>0.02</v>
@@ -9373,19 +9373,19 @@
         <v>0.03</v>
       </c>
       <c r="H128" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="I128" t="n">
-        <v>-33.333336</v>
+        <v>0</v>
       </c>
       <c r="J128" t="n">
-        <v>4037</v>
+        <v>4058</v>
       </c>
       <c r="K128" t="n">
         <v>6800</v>
       </c>
       <c r="L128" t="n">
-        <v>0.127938408203125</v>
+        <v>0.125985302734375</v>
       </c>
       <c r="M128" t="b">
         <v>0</v>
@@ -9449,13 +9449,13 @@
         <v>0</v>
       </c>
       <c r="J129" t="n">
-        <v>1160</v>
+        <v>1169</v>
       </c>
       <c r="K129" t="n">
         <v>5261</v>
       </c>
       <c r="L129" t="n">
-        <v>0.132821171875</v>
+        <v>0.13086806640625</v>
       </c>
       <c r="M129" t="b">
         <v>0</v>
@@ -9504,7 +9504,7 @@
         <v>448</v>
       </c>
       <c r="E130" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F130" t="n">
         <v>0.01</v>
@@ -9513,19 +9513,19 @@
         <v>0.02</v>
       </c>
       <c r="H130" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="I130" t="n">
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="J130" t="n">
-        <v>1225</v>
+        <v>1263</v>
       </c>
       <c r="K130" t="n">
         <v>5857</v>
       </c>
       <c r="L130" t="n">
-        <v>0.1445398046875</v>
+        <v>0.14258669921875</v>
       </c>
       <c r="M130" t="b">
         <v>0</v>
@@ -9595,7 +9595,7 @@
         <v>4764</v>
       </c>
       <c r="L131" t="n">
-        <v>0.1445398046875</v>
+        <v>0.14063359375</v>
       </c>
       <c r="M131" t="b">
         <v>0</v>
@@ -9623,7 +9623,7 @@
         <v>0</v>
       </c>
       <c r="T131" t="n">
-        <v>-0.002</v>
+        <v>-0.001</v>
       </c>
     </row>
     <row r="132">
@@ -9659,7 +9659,7 @@
         <v>0</v>
       </c>
       <c r="J132" t="n">
-        <v>1488</v>
+        <v>1494</v>
       </c>
       <c r="K132" t="n">
         <v>34672</v>
@@ -9693,7 +9693,7 @@
         <v>0</v>
       </c>
       <c r="T132" t="n">
-        <v>-0.001</v>
+        <v>-0.002</v>
       </c>
     </row>
     <row r="133">
@@ -9763,7 +9763,7 @@
         <v>0</v>
       </c>
       <c r="T133" t="n">
-        <v>-0.001</v>
+        <v>-0.002</v>
       </c>
     </row>
     <row r="134">
@@ -9805,7 +9805,7 @@
         <v>8042</v>
       </c>
       <c r="L134" t="n">
-        <v>0.1757894921875</v>
+        <v>0.17188328125</v>
       </c>
       <c r="M134" t="b">
         <v>0</v>
@@ -10015,7 +10015,7 @@
         <v>15026</v>
       </c>
       <c r="L137" t="n">
-        <v>0.2070391796875</v>
+        <v>0.20313296875</v>
       </c>
       <c r="M137" t="b">
         <v>0</v>
@@ -10155,7 +10155,7 @@
         <v>256</v>
       </c>
       <c r="L139" t="n">
-        <v>0.226570234375</v>
+        <v>0.2226640234375</v>
       </c>
       <c r="M139" t="b">
         <v>0</v>
@@ -10295,7 +10295,7 @@
         <v>377</v>
       </c>
       <c r="L141" t="n">
-        <v>0.2461012890625</v>
+        <v>0.242195078125</v>
       </c>
       <c r="M141" t="b">
         <v>0</v>
@@ -10365,7 +10365,7 @@
         <v>70387</v>
       </c>
       <c r="L142" t="n">
-        <v>0.257819921875</v>
+        <v>0.2539137109375</v>
       </c>
       <c r="M142" t="b">
         <v>0</v>
@@ -10505,7 +10505,7 @@
         <v>2740</v>
       </c>
       <c r="L144" t="n">
-        <v>0.29688203125</v>
+        <v>0.2929758203124999</v>
       </c>
       <c r="M144" t="b">
         <v>0</v>
@@ -10715,7 +10715,7 @@
         <v>531</v>
       </c>
       <c r="L147" t="n">
-        <v>0.3320379296875</v>
+        <v>0.32813171875</v>
       </c>
       <c r="M147" t="b">
         <v>0</v>
@@ -10925,7 +10925,7 @@
         <v>267</v>
       </c>
       <c r="L150" t="n">
-        <v>0.39063109375</v>
+        <v>0.3867248828124999</v>
       </c>
       <c r="M150" t="b">
         <v>0</v>
@@ -11203,7 +11203,7 @@
         <v>3662</v>
       </c>
       <c r="L154" t="n">
-        <v>0.445318046875</v>
+        <v>0.437505625</v>
       </c>
       <c r="M154" t="b">
         <v>0</v>
@@ -11833,7 +11833,7 @@
         <v>19758</v>
       </c>
       <c r="L163" t="n">
-        <v>0.7812521875</v>
+        <v>0.7656273437500001</v>
       </c>
       <c r="M163" t="b">
         <v>0</v>
@@ -11903,7 +11903,7 @@
         <v>688</v>
       </c>
       <c r="L164" t="n">
-        <v>0.85937640625</v>
+        <v>0.851563984375</v>
       </c>
       <c r="M164" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added a column to tract the return up untill 12:30
</commit_message>
<xml_diff>
--- a/calls_output.xlsx
+++ b/calls_output.xlsx
@@ -551,10 +551,10 @@
         <v>182.25</v>
       </c>
       <c r="F2" t="n">
-        <v>182.01</v>
+        <v>182.42</v>
       </c>
       <c r="G2" t="n">
-        <v>182.26</v>
+        <v>182.68</v>
       </c>
       <c r="H2" t="n">
         <v>0.5299988</v>
@@ -691,10 +691,10 @@
         <v>166.37</v>
       </c>
       <c r="F4" t="n">
-        <v>172.04</v>
+        <v>172.45</v>
       </c>
       <c r="G4" t="n">
-        <v>172.3</v>
+        <v>172.7</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>1e-05</v>
+        <v>2.1250046875</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -761,10 +761,10 @@
         <v>169.74</v>
       </c>
       <c r="F5" t="n">
-        <v>167.04</v>
+        <v>167.55</v>
       </c>
       <c r="G5" t="n">
-        <v>167.3</v>
+        <v>167.89</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -779,7 +779,7 @@
         <v>4</v>
       </c>
       <c r="L5" t="n">
-        <v>1e-05</v>
+        <v>2.24219189453125</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
@@ -807,7 +807,7 @@
         <v>0.007</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.039</v>
+        <v>-0.041</v>
       </c>
     </row>
     <row r="6">
@@ -831,10 +831,10 @@
         <v>166.53</v>
       </c>
       <c r="F6" t="n">
-        <v>162.11</v>
+        <v>162.48</v>
       </c>
       <c r="G6" t="n">
-        <v>162.38</v>
+        <v>162.72</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -849,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>1e-05</v>
+        <v>2.16406708984375</v>
       </c>
       <c r="M6" t="b">
         <v>1</v>
@@ -877,7 +877,7 @@
         <v>0.008</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.04</v>
+        <v>-0.041</v>
       </c>
     </row>
     <row r="7">
@@ -901,10 +901,10 @@
         <v>160.69</v>
       </c>
       <c r="F7" t="n">
-        <v>157.04</v>
+        <v>157.54</v>
       </c>
       <c r="G7" t="n">
-        <v>157.29</v>
+        <v>157.9</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -919,7 +919,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1e-05</v>
+        <v>2.085942285156249</v>
       </c>
       <c r="M7" t="b">
         <v>1</v>
@@ -947,7 +947,7 @@
         <v>0.008</v>
       </c>
       <c r="T7" t="n">
-        <v>-0.04</v>
+        <v>-0.042</v>
       </c>
     </row>
     <row r="8">
@@ -971,10 +971,10 @@
         <v>156.53</v>
       </c>
       <c r="F8" t="n">
-        <v>152.06</v>
+        <v>152.48</v>
       </c>
       <c r="G8" t="n">
-        <v>152.3</v>
+        <v>152.74</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -989,7 +989,7 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>1e-05</v>
+        <v>2.1093797265625</v>
       </c>
       <c r="M8" t="b">
         <v>1</v>
@@ -1017,7 +1017,7 @@
         <v>0.008</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.041</v>
+        <v>-0.045</v>
       </c>
     </row>
     <row r="9">
@@ -1111,10 +1111,10 @@
         <v>127.3</v>
       </c>
       <c r="F10" t="n">
-        <v>142.15</v>
+        <v>142.46</v>
       </c>
       <c r="G10" t="n">
-        <v>142.38</v>
+        <v>142.86</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1129,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>1e-05</v>
+        <v>2.236332534179687</v>
       </c>
       <c r="M10" t="b">
         <v>1</v>
@@ -1157,7 +1157,7 @@
         <v>0.008</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.042</v>
+        <v>-0.07099999999999999</v>
       </c>
     </row>
     <row r="11">
@@ -1181,10 +1181,10 @@
         <v>134.86</v>
       </c>
       <c r="F11" t="n">
-        <v>137.07</v>
+        <v>137.49</v>
       </c>
       <c r="G11" t="n">
-        <v>137.31</v>
+        <v>137.75</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1199,7 +1199,7 @@
         <v>12</v>
       </c>
       <c r="L11" t="n">
-        <v>1e-05</v>
+        <v>1.9140629296875</v>
       </c>
       <c r="M11" t="b">
         <v>1</v>
@@ -1227,7 +1227,7 @@
         <v>0.008</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.043</v>
+        <v>-0.049</v>
       </c>
     </row>
     <row r="12">
@@ -1251,10 +1251,10 @@
         <v>129.25</v>
       </c>
       <c r="F12" t="n">
-        <v>132.07</v>
+        <v>132.6</v>
       </c>
       <c r="G12" t="n">
-        <v>132.3</v>
+        <v>132.92</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1269,7 +1269,7 @@
         <v>4</v>
       </c>
       <c r="L12" t="n">
-        <v>1e-05</v>
+        <v>1.8671881640625</v>
       </c>
       <c r="M12" t="b">
         <v>1</v>
@@ -1297,7 +1297,7 @@
         <v>0.008</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.044</v>
+        <v>-0.052</v>
       </c>
     </row>
     <row r="13">
@@ -1321,10 +1321,10 @@
         <v>121.41</v>
       </c>
       <c r="F13" t="n">
-        <v>127.1</v>
+        <v>127.52</v>
       </c>
       <c r="G13" t="n">
-        <v>127.38</v>
+        <v>127.8</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1339,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>1e-05</v>
+        <v>1.87890685546875</v>
       </c>
       <c r="M13" t="b">
         <v>1</v>
@@ -1367,7 +1367,7 @@
         <v>0.008</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.045</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="14">
@@ -1391,10 +1391,10 @@
         <v>122.01</v>
       </c>
       <c r="F14" t="n">
-        <v>122.08</v>
+        <v>122.49</v>
       </c>
       <c r="G14" t="n">
-        <v>122.32</v>
+        <v>122.74</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1409,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>1e-05</v>
+        <v>1.65234548828125</v>
       </c>
       <c r="M14" t="b">
         <v>1</v>
@@ -1437,7 +1437,7 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.045</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="15">
@@ -1461,10 +1461,10 @@
         <v>114.84</v>
       </c>
       <c r="F15" t="n">
-        <v>117.08</v>
+        <v>117.51</v>
       </c>
       <c r="G15" t="n">
-        <v>117.31</v>
+        <v>117.75</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1479,7 +1479,7 @@
         <v>12</v>
       </c>
       <c r="L15" t="n">
-        <v>1e-05</v>
+        <v>1.609376953125</v>
       </c>
       <c r="M15" t="b">
         <v>1</v>
@@ -1507,7 +1507,7 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="T15" t="n">
-        <v>-0.046</v>
+        <v>-0.052</v>
       </c>
     </row>
     <row r="16">
@@ -1531,10 +1531,10 @@
         <v>111.8</v>
       </c>
       <c r="F16" t="n">
-        <v>112.15</v>
+        <v>112.55</v>
       </c>
       <c r="G16" t="n">
-        <v>112.41</v>
+        <v>112.8</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1549,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>1e-05</v>
+        <v>1.646486142578125</v>
       </c>
       <c r="M16" t="b">
         <v>1</v>
@@ -1577,7 +1577,7 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.047</v>
+        <v>-0.063</v>
       </c>
     </row>
     <row r="17">
@@ -1601,10 +1601,10 @@
         <v>103.11</v>
       </c>
       <c r="F17" t="n">
-        <v>107.16</v>
+        <v>107.62</v>
       </c>
       <c r="G17" t="n">
-        <v>107.37</v>
+        <v>107.88</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1619,7 +1619,7 @@
         <v>6</v>
       </c>
       <c r="L17" t="n">
-        <v>1e-05</v>
+        <v>1.46484642578125</v>
       </c>
       <c r="M17" t="b">
         <v>1</v>
@@ -1647,7 +1647,7 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.047</v>
+        <v>-0.054</v>
       </c>
     </row>
     <row r="18">
@@ -1671,10 +1671,10 @@
         <v>99.83</v>
       </c>
       <c r="F18" t="n">
-        <v>102.09</v>
+        <v>102.62</v>
       </c>
       <c r="G18" t="n">
-        <v>102.33</v>
+        <v>102.89</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1689,7 +1689,7 @@
         <v>20</v>
       </c>
       <c r="L18" t="n">
-        <v>1e-05</v>
+        <v>1.40625296875</v>
       </c>
       <c r="M18" t="b">
         <v>1</v>
@@ -1717,7 +1717,7 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.048</v>
+        <v>-0.056</v>
       </c>
     </row>
     <row r="19">
@@ -1741,10 +1741,10 @@
         <v>100.75</v>
       </c>
       <c r="F19" t="n">
-        <v>100.16</v>
+        <v>100.48</v>
       </c>
       <c r="G19" t="n">
-        <v>100.38</v>
+        <v>100.73</v>
       </c>
       <c r="H19" t="n">
         <v>4.5699997</v>
@@ -1759,7 +1759,7 @@
         <v>1</v>
       </c>
       <c r="L19" t="n">
-        <v>1e-05</v>
+        <v>1.3125034375</v>
       </c>
       <c r="M19" t="b">
         <v>1</v>
@@ -1787,7 +1787,7 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="T19" t="n">
-        <v>-0.048</v>
+        <v>-0.052</v>
       </c>
     </row>
     <row r="20">
@@ -1811,10 +1811,10 @@
         <v>95.20999999999999</v>
       </c>
       <c r="F20" t="n">
-        <v>99.16</v>
+        <v>99.69</v>
       </c>
       <c r="G20" t="n">
-        <v>99.42</v>
+        <v>99.95</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -1829,7 +1829,7 @@
         <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>1e-05</v>
+        <v>1.48047134765625</v>
       </c>
       <c r="M20" t="b">
         <v>1</v>
@@ -1857,7 +1857,7 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="T20" t="n">
-        <v>-0.049</v>
+        <v>-0.07099999999999999</v>
       </c>
     </row>
     <row r="21">
@@ -1881,10 +1881,10 @@
         <v>98.77</v>
       </c>
       <c r="F21" t="n">
-        <v>98.11</v>
+        <v>98.51000000000001</v>
       </c>
       <c r="G21" t="n">
-        <v>98.39</v>
+        <v>98.76000000000001</v>
       </c>
       <c r="H21" t="n">
         <v>14.119995</v>
@@ -1899,7 +1899,7 @@
         <v>2</v>
       </c>
       <c r="L21" t="n">
-        <v>1e-05</v>
+        <v>1.36328443359375</v>
       </c>
       <c r="M21" t="b">
         <v>1</v>
@@ -1927,7 +1927,7 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="T21" t="n">
-        <v>-0.049</v>
+        <v>-0.058</v>
       </c>
     </row>
     <row r="22">
@@ -1951,10 +1951,10 @@
         <v>96.63</v>
       </c>
       <c r="F22" t="n">
-        <v>97.11</v>
+        <v>97.51000000000001</v>
       </c>
       <c r="G22" t="n">
-        <v>97.39</v>
+        <v>97.76000000000001</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1969,7 +1969,7 @@
         <v>7</v>
       </c>
       <c r="L22" t="n">
-        <v>1e-05</v>
+        <v>1.34765951171875</v>
       </c>
       <c r="M22" t="b">
         <v>1</v>
@@ -1997,7 +1997,7 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="T22" t="n">
-        <v>-0.049</v>
+        <v>-0.058</v>
       </c>
     </row>
     <row r="23">
@@ -2299,10 +2299,10 @@
         <v>97.31999999999999</v>
       </c>
       <c r="F27" t="n">
-        <v>92.17</v>
+        <v>92.63</v>
       </c>
       <c r="G27" t="n">
-        <v>92.38</v>
+        <v>92.89</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -2317,7 +2317,7 @@
         <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>1e-05</v>
+        <v>1.27734736328125</v>
       </c>
       <c r="M27" t="b">
         <v>1</v>
@@ -2345,7 +2345,7 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="T27" t="n">
-        <v>-0.05</v>
+        <v>-0.059</v>
       </c>
     </row>
     <row r="28">
@@ -2577,10 +2577,10 @@
         <v>93.37</v>
       </c>
       <c r="F31" t="n">
-        <v>88.13</v>
+        <v>88.59999999999999</v>
       </c>
       <c r="G31" t="n">
-        <v>88.34999999999999</v>
+        <v>88.90000000000001</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -2595,7 +2595,7 @@
         <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>1e-05</v>
+        <v>1.19922275390625</v>
       </c>
       <c r="M31" t="b">
         <v>1</v>
@@ -2623,7 +2623,7 @@
         <v>0.01</v>
       </c>
       <c r="T31" t="n">
-        <v>-0.05</v>
+        <v>-0.057</v>
       </c>
     </row>
     <row r="32">
@@ -2644,28 +2644,28 @@
         <v>350</v>
       </c>
       <c r="E32" t="n">
-        <v>87.59</v>
+        <v>87.61</v>
       </c>
       <c r="F32" t="n">
-        <v>87.09</v>
+        <v>87.55</v>
       </c>
       <c r="G32" t="n">
-        <v>87.34999999999999</v>
+        <v>87.84</v>
       </c>
       <c r="H32" t="n">
-        <v>1.6299973</v>
+        <v>1.6500015</v>
       </c>
       <c r="I32" t="n">
-        <v>1.8962276</v>
+        <v>1.9194993</v>
       </c>
       <c r="J32" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K32" t="n">
         <v>46</v>
       </c>
       <c r="L32" t="n">
-        <v>1e-05</v>
+        <v>0.937500625</v>
       </c>
       <c r="M32" t="b">
         <v>1</v>
@@ -2717,10 +2717,10 @@
         <v>79.75</v>
       </c>
       <c r="F33" t="n">
-        <v>86.17</v>
+        <v>86.52</v>
       </c>
       <c r="G33" t="n">
-        <v>86.39</v>
+        <v>86.77</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -2735,7 +2735,7 @@
         <v>2</v>
       </c>
       <c r="L33" t="n">
-        <v>1e-05</v>
+        <v>1.2109414453125</v>
       </c>
       <c r="M33" t="b">
         <v>1</v>
@@ -2763,7 +2763,7 @@
         <v>0.01</v>
       </c>
       <c r="T33" t="n">
-        <v>-0.05</v>
+        <v>-0.062</v>
       </c>
     </row>
     <row r="34">
@@ -2787,10 +2787,10 @@
         <v>90.48999999999999</v>
       </c>
       <c r="F34" t="n">
-        <v>85.17</v>
+        <v>85.64</v>
       </c>
       <c r="G34" t="n">
-        <v>85.43000000000001</v>
+        <v>85.84999999999999</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -2805,7 +2805,7 @@
         <v>1</v>
       </c>
       <c r="L34" t="n">
-        <v>1e-05</v>
+        <v>1.1484417578125</v>
       </c>
       <c r="M34" t="b">
         <v>1</v>
@@ -2833,7 +2833,7 @@
         <v>0.01</v>
       </c>
       <c r="T34" t="n">
-        <v>-0.051</v>
+        <v>-0.057</v>
       </c>
     </row>
     <row r="35">
@@ -2857,10 +2857,10 @@
         <v>75.52</v>
       </c>
       <c r="F35" t="n">
-        <v>84.12</v>
+        <v>84.52</v>
       </c>
       <c r="G35" t="n">
-        <v>84.40000000000001</v>
+        <v>84.77</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
@@ -2875,7 +2875,7 @@
         <v>0</v>
       </c>
       <c r="L35" t="n">
-        <v>1e-05</v>
+        <v>1.18359783203125</v>
       </c>
       <c r="M35" t="b">
         <v>1</v>
@@ -2903,7 +2903,7 @@
         <v>0.01</v>
       </c>
       <c r="T35" t="n">
-        <v>-0.051</v>
+        <v>-0.062</v>
       </c>
     </row>
     <row r="36">
@@ -2945,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="L36" t="n">
-        <v>2.199711531982421</v>
+        <v>2.166752630004883</v>
       </c>
       <c r="M36" t="b">
         <v>1</v>
@@ -2961,19 +2961,19 @@
         </is>
       </c>
       <c r="P36" t="n">
-        <v>0.971</v>
+        <v>0.973</v>
       </c>
       <c r="Q36" t="n">
         <v>0.001</v>
       </c>
       <c r="R36" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="S36" t="n">
         <v>0.008999999999999999</v>
       </c>
       <c r="T36" t="n">
-        <v>-1.706</v>
+        <v>-1.591</v>
       </c>
     </row>
     <row r="37">
@@ -2997,10 +2997,10 @@
         <v>88.51000000000001</v>
       </c>
       <c r="F37" t="n">
-        <v>82.11</v>
+        <v>82.56</v>
       </c>
       <c r="G37" t="n">
-        <v>82.34999999999999</v>
+        <v>82.83</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -3015,7 +3015,7 @@
         <v>5</v>
       </c>
       <c r="L37" t="n">
-        <v>1e-05</v>
+        <v>0.87500125</v>
       </c>
       <c r="M37" t="b">
         <v>1</v>
@@ -3067,10 +3067,10 @@
         <v>81.72</v>
       </c>
       <c r="F38" t="n">
-        <v>81.11</v>
+        <v>81.52</v>
       </c>
       <c r="G38" t="n">
-        <v>81.34999999999999</v>
+        <v>81.77</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -3085,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="L38" t="n">
-        <v>1e-05</v>
+        <v>1.142582412109375</v>
       </c>
       <c r="M38" t="b">
         <v>1</v>
@@ -3113,7 +3113,7 @@
         <v>0.01</v>
       </c>
       <c r="T38" t="n">
-        <v>-0.051</v>
+        <v>-0.063</v>
       </c>
     </row>
     <row r="39">
@@ -3207,10 +3207,10 @@
         <v>64.67</v>
       </c>
       <c r="F40" t="n">
-        <v>79.18000000000001</v>
+        <v>79.64</v>
       </c>
       <c r="G40" t="n">
-        <v>79.39</v>
+        <v>79.90000000000001</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -3225,7 +3225,7 @@
         <v>0</v>
       </c>
       <c r="L40" t="n">
-        <v>1e-05</v>
+        <v>1.11328568359375</v>
       </c>
       <c r="M40" t="b">
         <v>1</v>
@@ -3253,7 +3253,7 @@
         <v>0.01</v>
       </c>
       <c r="T40" t="n">
-        <v>-0.051</v>
+        <v>-0.063</v>
       </c>
     </row>
     <row r="41">
@@ -3347,10 +3347,10 @@
         <v>75.97</v>
       </c>
       <c r="F42" t="n">
-        <v>77.09999999999999</v>
+        <v>77.56</v>
       </c>
       <c r="G42" t="n">
-        <v>77.34</v>
+        <v>77.83</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -3365,7 +3365,7 @@
         <v>17</v>
       </c>
       <c r="L42" t="n">
-        <v>1e-05</v>
+        <v>0.8281267187499999</v>
       </c>
       <c r="M42" t="b">
         <v>1</v>
@@ -3627,10 +3627,10 @@
         <v>78.45999999999999</v>
       </c>
       <c r="F46" t="n">
-        <v>73.09999999999999</v>
+        <v>73.53</v>
       </c>
       <c r="G46" t="n">
-        <v>73.34</v>
+        <v>73.78</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -3645,7 +3645,7 @@
         <v>1</v>
       </c>
       <c r="L46" t="n">
-        <v>1e-05</v>
+        <v>1.046879765625</v>
       </c>
       <c r="M46" t="b">
         <v>1</v>
@@ -3673,7 +3673,7 @@
         <v>0.01</v>
       </c>
       <c r="T46" t="n">
-        <v>-0.052</v>
+        <v>-0.067</v>
       </c>
     </row>
     <row r="47">
@@ -3697,10 +3697,10 @@
         <v>67.95999999999999</v>
       </c>
       <c r="F47" t="n">
-        <v>72.09999999999999</v>
+        <v>72.55</v>
       </c>
       <c r="G47" t="n">
-        <v>72.34</v>
+        <v>72.84</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -3715,7 +3715,7 @@
         <v>15</v>
       </c>
       <c r="L47" t="n">
-        <v>1e-05</v>
+        <v>0.7812521875</v>
       </c>
       <c r="M47" t="b">
         <v>1</v>
@@ -3743,7 +3743,7 @@
         <v>0.01</v>
       </c>
       <c r="T47" t="n">
-        <v>-0.052</v>
+        <v>-0.053</v>
       </c>
     </row>
     <row r="48">
@@ -3767,10 +3767,10 @@
         <v>71.03</v>
       </c>
       <c r="F48" t="n">
-        <v>71.13</v>
+        <v>71.53</v>
       </c>
       <c r="G48" t="n">
-        <v>71.41</v>
+        <v>71.78</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -3785,7 +3785,7 @@
         <v>2</v>
       </c>
       <c r="L48" t="n">
-        <v>1e-05</v>
+        <v>1.01953615234375</v>
       </c>
       <c r="M48" t="b">
         <v>1</v>
@@ -3813,7 +3813,7 @@
         <v>0.01</v>
       </c>
       <c r="T48" t="n">
-        <v>-0.053</v>
+        <v>-0.068</v>
       </c>
     </row>
     <row r="49">
@@ -3855,7 +3855,7 @@
         <v>13</v>
       </c>
       <c r="L49" t="n">
-        <v>0.8281267187499999</v>
+        <v>1.126957490234375</v>
       </c>
       <c r="M49" t="b">
         <v>1</v>
@@ -3871,19 +3871,19 @@
         </is>
       </c>
       <c r="P49" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q49" t="n">
         <v>0</v>
       </c>
       <c r="R49" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S49" t="n">
         <v>0.01</v>
       </c>
       <c r="T49" t="n">
-        <v>-0.054</v>
+        <v>-0.107</v>
       </c>
     </row>
     <row r="50">
@@ -3907,10 +3907,10 @@
         <v>68.55</v>
       </c>
       <c r="F50" t="n">
-        <v>69.11</v>
+        <v>69.56999999999999</v>
       </c>
       <c r="G50" t="n">
-        <v>69.34</v>
+        <v>69.84</v>
       </c>
       <c r="H50" t="n">
         <v>0</v>
@@ -3925,7 +3925,7 @@
         <v>3</v>
       </c>
       <c r="L50" t="n">
-        <v>1e-05</v>
+        <v>0.8125018749999999</v>
       </c>
       <c r="M50" t="b">
         <v>1</v>
@@ -3953,7 +3953,7 @@
         <v>0.01</v>
       </c>
       <c r="T50" t="n">
-        <v>-0.053</v>
+        <v>-0.054</v>
       </c>
     </row>
     <row r="51">
@@ -3977,10 +3977,10 @@
         <v>73.09</v>
       </c>
       <c r="F51" t="n">
-        <v>68.11</v>
+        <v>68.65000000000001</v>
       </c>
       <c r="G51" t="n">
-        <v>68.37</v>
+        <v>68.91</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -3995,7 +3995,7 @@
         <v>2</v>
       </c>
       <c r="L51" t="n">
-        <v>1e-05</v>
+        <v>0.9785158398437501</v>
       </c>
       <c r="M51" t="b">
         <v>1</v>
@@ -4023,7 +4023,7 @@
         <v>0.01</v>
       </c>
       <c r="T51" t="n">
-        <v>-0.053</v>
+        <v>-0.06900000000000001</v>
       </c>
     </row>
     <row r="52">
@@ -4044,28 +4044,28 @@
         <v>370</v>
       </c>
       <c r="E52" t="n">
-        <v>65.95999999999999</v>
+        <v>67.66</v>
       </c>
       <c r="F52" t="n">
-        <v>67.11</v>
+        <v>67.65000000000001</v>
       </c>
       <c r="G52" t="n">
-        <v>67.36</v>
+        <v>67.91</v>
       </c>
       <c r="H52" t="n">
-        <v>0</v>
+        <v>1.7000046</v>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>2.5773265</v>
       </c>
       <c r="J52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K52" t="n">
         <v>34</v>
       </c>
       <c r="L52" t="n">
-        <v>1e-05</v>
+        <v>0.9648441015625</v>
       </c>
       <c r="M52" t="b">
         <v>1</v>
@@ -4093,7 +4093,7 @@
         <v>0.01</v>
       </c>
       <c r="T52" t="n">
-        <v>-0.053</v>
+        <v>-0.06900000000000001</v>
       </c>
     </row>
     <row r="53">
@@ -4117,10 +4117,10 @@
         <v>72.03</v>
       </c>
       <c r="F53" t="n">
-        <v>66.19</v>
+        <v>66.65000000000001</v>
       </c>
       <c r="G53" t="n">
-        <v>66.40000000000001</v>
+        <v>66.91</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -4135,7 +4135,7 @@
         <v>0</v>
       </c>
       <c r="L53" t="n">
-        <v>1e-05</v>
+        <v>0.9511723632812499</v>
       </c>
       <c r="M53" t="b">
         <v>1</v>
@@ -4163,7 +4163,7 @@
         <v>0.01</v>
       </c>
       <c r="T53" t="n">
-        <v>-0.053</v>
+        <v>-0.06900000000000001</v>
       </c>
     </row>
     <row r="54">
@@ -4257,10 +4257,10 @@
         <v>63.18</v>
       </c>
       <c r="F55" t="n">
-        <v>64.11</v>
+        <v>64.56999999999999</v>
       </c>
       <c r="G55" t="n">
-        <v>64.34999999999999</v>
+        <v>64.84</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -4275,7 +4275,7 @@
         <v>2</v>
       </c>
       <c r="L55" t="n">
-        <v>1e-05</v>
+        <v>0.7578149218750001</v>
       </c>
       <c r="M55" t="b">
         <v>1</v>
@@ -4303,7 +4303,7 @@
         <v>0.01</v>
       </c>
       <c r="T55" t="n">
-        <v>-0.054</v>
+        <v>-0.055</v>
       </c>
     </row>
     <row r="56">
@@ -4327,10 +4327,10 @@
         <v>49.11</v>
       </c>
       <c r="F56" t="n">
-        <v>63.13</v>
+        <v>63.66</v>
       </c>
       <c r="G56" t="n">
-        <v>63.35</v>
+        <v>63.98</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -4345,7 +4345,7 @@
         <v>0</v>
       </c>
       <c r="L56" t="n">
-        <v>1e-05</v>
+        <v>0.95507857421875</v>
       </c>
       <c r="M56" t="b">
         <v>1</v>
@@ -4361,19 +4361,19 @@
         </is>
       </c>
       <c r="P56" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q56" t="n">
         <v>0</v>
       </c>
       <c r="R56" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S56" t="n">
         <v>0.01</v>
       </c>
       <c r="T56" t="n">
-        <v>-0.054</v>
+        <v>-0.082</v>
       </c>
     </row>
     <row r="57">
@@ -4397,10 +4397,10 @@
         <v>68.31</v>
       </c>
       <c r="F57" t="n">
-        <v>62.11</v>
+        <v>62.54</v>
       </c>
       <c r="G57" t="n">
-        <v>62.37</v>
+        <v>62.79</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -4415,7 +4415,7 @@
         <v>3</v>
       </c>
       <c r="L57" t="n">
-        <v>1e-05</v>
+        <v>0.9082040429687499</v>
       </c>
       <c r="M57" t="b">
         <v>1</v>
@@ -4431,7 +4431,7 @@
         </is>
       </c>
       <c r="P57" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q57" t="n">
         <v>0</v>
@@ -4443,7 +4443,7 @@
         <v>0.01</v>
       </c>
       <c r="T57" t="n">
-        <v>-0.054</v>
+        <v>-0.073</v>
       </c>
     </row>
     <row r="58">
@@ -4467,10 +4467,10 @@
         <v>60.19</v>
       </c>
       <c r="F58" t="n">
-        <v>61.13</v>
+        <v>61.72</v>
       </c>
       <c r="G58" t="n">
-        <v>61.36</v>
+        <v>61.92</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -4485,7 +4485,7 @@
         <v>1</v>
       </c>
       <c r="L58" t="n">
-        <v>1e-05</v>
+        <v>0.9257819921875</v>
       </c>
       <c r="M58" t="b">
         <v>1</v>
@@ -4501,19 +4501,19 @@
         </is>
       </c>
       <c r="P58" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q58" t="n">
         <v>0</v>
       </c>
       <c r="R58" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S58" t="n">
         <v>0.01</v>
       </c>
       <c r="T58" t="n">
-        <v>-0.054</v>
+        <v>-0.083</v>
       </c>
     </row>
     <row r="59">
@@ -4537,10 +4537,10 @@
         <v>59.51</v>
       </c>
       <c r="F59" t="n">
-        <v>60.11</v>
+        <v>60.64</v>
       </c>
       <c r="G59" t="n">
-        <v>60.35</v>
+        <v>60.87</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -4555,7 +4555,7 @@
         <v>0</v>
       </c>
       <c r="L59" t="n">
-        <v>1e-05</v>
+        <v>0.8339860351562498</v>
       </c>
       <c r="M59" t="b">
         <v>1</v>
@@ -4583,7 +4583,7 @@
         <v>0.01</v>
       </c>
       <c r="T59" t="n">
-        <v>-0.054</v>
+        <v>-0.064</v>
       </c>
     </row>
     <row r="60">
@@ -4607,10 +4607,10 @@
         <v>58.56</v>
       </c>
       <c r="F60" t="n">
-        <v>59.12</v>
+        <v>59.66</v>
       </c>
       <c r="G60" t="n">
-        <v>59.35</v>
+        <v>59.89</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -4625,7 +4625,7 @@
         <v>2</v>
       </c>
       <c r="L60" t="n">
-        <v>1e-05</v>
+        <v>0.8476577734374999</v>
       </c>
       <c r="M60" t="b">
         <v>1</v>
@@ -4653,7 +4653,7 @@
         <v>0.01</v>
       </c>
       <c r="T60" t="n">
-        <v>-0.054</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="61">
@@ -4677,10 +4677,10 @@
         <v>57.86</v>
       </c>
       <c r="F61" t="n">
-        <v>58.1</v>
+        <v>58.65</v>
       </c>
       <c r="G61" t="n">
-        <v>58.34</v>
+        <v>58.89</v>
       </c>
       <c r="H61" t="n">
         <v>0.3199997</v>
@@ -4695,7 +4695,7 @@
         <v>1</v>
       </c>
       <c r="L61" t="n">
-        <v>1e-05</v>
+        <v>0.8281267187499999</v>
       </c>
       <c r="M61" t="b">
         <v>1</v>
@@ -4723,7 +4723,7 @@
         <v>0.01</v>
       </c>
       <c r="T61" t="n">
-        <v>-0.055</v>
+        <v>-0.06900000000000001</v>
       </c>
     </row>
     <row r="62">
@@ -4747,10 +4747,10 @@
         <v>57.38</v>
       </c>
       <c r="F62" t="n">
-        <v>57.16</v>
+        <v>57.54</v>
       </c>
       <c r="G62" t="n">
-        <v>57.46</v>
+        <v>57.79</v>
       </c>
       <c r="H62" t="n">
         <v>1.5400009</v>
@@ -4765,7 +4765,7 @@
         <v>68</v>
       </c>
       <c r="L62" t="n">
-        <v>1e-05</v>
+        <v>0.8398453515625</v>
       </c>
       <c r="M62" t="b">
         <v>1</v>
@@ -4781,7 +4781,7 @@
         </is>
       </c>
       <c r="P62" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q62" t="n">
         <v>0</v>
@@ -4793,7 +4793,7 @@
         <v>0.01</v>
       </c>
       <c r="T62" t="n">
-        <v>-0.055</v>
+        <v>-0.075</v>
       </c>
     </row>
     <row r="63">
@@ -4817,10 +4817,10 @@
         <v>49.22</v>
       </c>
       <c r="F63" t="n">
-        <v>56.16</v>
+        <v>56.76</v>
       </c>
       <c r="G63" t="n">
-        <v>56.39</v>
+        <v>57.03</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -4835,7 +4835,7 @@
         <v>0</v>
       </c>
       <c r="L63" t="n">
-        <v>1e-05</v>
+        <v>0.9140633593750001</v>
       </c>
       <c r="M63" t="b">
         <v>1</v>
@@ -4851,19 +4851,19 @@
         </is>
       </c>
       <c r="P63" t="n">
-        <v>1</v>
+        <v>0.998</v>
       </c>
       <c r="Q63" t="n">
         <v>0</v>
       </c>
       <c r="R63" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S63" t="n">
         <v>0.01</v>
       </c>
       <c r="T63" t="n">
-        <v>-0.055</v>
+        <v>-0.113</v>
       </c>
     </row>
     <row r="64">
@@ -4887,10 +4887,10 @@
         <v>58.71</v>
       </c>
       <c r="F64" t="n">
-        <v>55.13</v>
+        <v>55.56</v>
       </c>
       <c r="G64" t="n">
-        <v>55.38</v>
+        <v>55.79</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -4905,7 +4905,7 @@
         <v>0</v>
       </c>
       <c r="L64" t="n">
-        <v>1e-05</v>
+        <v>0.8125018749999999</v>
       </c>
       <c r="M64" t="b">
         <v>1</v>
@@ -4921,19 +4921,19 @@
         </is>
       </c>
       <c r="P64" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q64" t="n">
         <v>0</v>
       </c>
       <c r="R64" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S64" t="n">
         <v>0.01</v>
       </c>
       <c r="T64" t="n">
-        <v>-0.055</v>
+        <v>-0.075</v>
       </c>
     </row>
     <row r="65">
@@ -4957,10 +4957,10 @@
         <v>59.92</v>
       </c>
       <c r="F65" t="n">
-        <v>54.2</v>
+        <v>54.66</v>
       </c>
       <c r="G65" t="n">
-        <v>54.41</v>
+        <v>54.92</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -4975,7 +4975,7 @@
         <v>0</v>
       </c>
       <c r="L65" t="n">
-        <v>1e-05</v>
+        <v>0.79883013671875</v>
       </c>
       <c r="M65" t="b">
         <v>1</v>
@@ -4991,19 +4991,19 @@
         </is>
       </c>
       <c r="P65" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q65" t="n">
         <v>0</v>
       </c>
       <c r="R65" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S65" t="n">
         <v>0.01</v>
       </c>
       <c r="T65" t="n">
-        <v>-0.055</v>
+        <v>-0.076</v>
       </c>
     </row>
     <row r="66">
@@ -5027,10 +5027,10 @@
         <v>58.15</v>
       </c>
       <c r="F66" t="n">
-        <v>53.2</v>
+        <v>53.57</v>
       </c>
       <c r="G66" t="n">
-        <v>53.41</v>
+        <v>53.82</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -5045,7 +5045,7 @@
         <v>1</v>
       </c>
       <c r="L66" t="n">
-        <v>1e-05</v>
+        <v>0.5625043750000001</v>
       </c>
       <c r="M66" t="b">
         <v>1</v>
@@ -5097,10 +5097,10 @@
         <v>51.46</v>
       </c>
       <c r="F67" t="n">
-        <v>52.14</v>
+        <v>52.67</v>
       </c>
       <c r="G67" t="n">
-        <v>52.36</v>
+        <v>52.93</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -5115,7 +5115,7 @@
         <v>21</v>
       </c>
       <c r="L67" t="n">
-        <v>1e-05</v>
+        <v>0.7812521875</v>
       </c>
       <c r="M67" t="b">
         <v>1</v>
@@ -5131,19 +5131,19 @@
         </is>
       </c>
       <c r="P67" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q67" t="n">
         <v>0</v>
       </c>
       <c r="R67" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S67" t="n">
         <v>0.011</v>
       </c>
       <c r="T67" t="n">
-        <v>-0.055</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="68">
@@ -5167,10 +5167,10 @@
         <v>50.32</v>
       </c>
       <c r="F68" t="n">
-        <v>51.14</v>
+        <v>51.63</v>
       </c>
       <c r="G68" t="n">
-        <v>51.37</v>
+        <v>51.93</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -5185,7 +5185,7 @@
         <v>1</v>
       </c>
       <c r="L68" t="n">
-        <v>1e-05</v>
+        <v>0.7460962890625</v>
       </c>
       <c r="M68" t="b">
         <v>1</v>
@@ -5201,7 +5201,7 @@
         </is>
       </c>
       <c r="P68" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q68" t="n">
         <v>0</v>
@@ -5213,7 +5213,7 @@
         <v>0.011</v>
       </c>
       <c r="T68" t="n">
-        <v>-0.056</v>
+        <v>-0.073</v>
       </c>
     </row>
     <row r="69">
@@ -5237,10 +5237,10 @@
         <v>49.56</v>
       </c>
       <c r="F69" t="n">
-        <v>50.23</v>
+        <v>50.65</v>
       </c>
       <c r="G69" t="n">
-        <v>50.48</v>
+        <v>50.8</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -5255,7 +5255,7 @@
         <v>5</v>
       </c>
       <c r="L69" t="n">
-        <v>1e-05</v>
+        <v>0.6523472265625001</v>
       </c>
       <c r="M69" t="b">
         <v>1</v>
@@ -5283,7 +5283,7 @@
         <v>0.011</v>
       </c>
       <c r="T69" t="n">
-        <v>-0.056</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="70">
@@ -5307,10 +5307,10 @@
         <v>54.01</v>
       </c>
       <c r="F70" t="n">
-        <v>49.12</v>
+        <v>49.77</v>
       </c>
       <c r="G70" t="n">
-        <v>49.36</v>
+        <v>49.88</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -5325,7 +5325,7 @@
         <v>0</v>
       </c>
       <c r="L70" t="n">
-        <v>1e-05</v>
+        <v>0.7617211328125001</v>
       </c>
       <c r="M70" t="b">
         <v>1</v>
@@ -5341,19 +5341,19 @@
         </is>
       </c>
       <c r="P70" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q70" t="n">
         <v>0</v>
       </c>
       <c r="R70" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S70" t="n">
         <v>0.011</v>
       </c>
       <c r="T70" t="n">
-        <v>-0.056</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="71">
@@ -5377,10 +5377,10 @@
         <v>46.92</v>
       </c>
       <c r="F71" t="n">
-        <v>48.13</v>
+        <v>48.67</v>
       </c>
       <c r="G71" t="n">
-        <v>48.36</v>
+        <v>48.88</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -5395,7 +5395,7 @@
         <v>2</v>
       </c>
       <c r="L71" t="n">
-        <v>1e-05</v>
+        <v>0.70117486328125</v>
       </c>
       <c r="M71" t="b">
         <v>1</v>
@@ -5411,7 +5411,7 @@
         </is>
       </c>
       <c r="P71" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q71" t="n">
         <v>0</v>
@@ -5423,7 +5423,7 @@
         <v>0.011</v>
       </c>
       <c r="T71" t="n">
-        <v>-0.056</v>
+        <v>-0.073</v>
       </c>
     </row>
     <row r="72">
@@ -5444,28 +5444,28 @@
         <v>390</v>
       </c>
       <c r="E72" t="n">
-        <v>46.01</v>
+        <v>47.5</v>
       </c>
       <c r="F72" t="n">
-        <v>47.11</v>
+        <v>47.45</v>
       </c>
       <c r="G72" t="n">
-        <v>47.35</v>
+        <v>47.99</v>
       </c>
       <c r="H72" t="n">
-        <v>0</v>
+        <v>1.4900017</v>
       </c>
       <c r="I72" t="n">
-        <v>0</v>
+        <v>3.2384303</v>
       </c>
       <c r="J72" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K72" t="n">
         <v>9</v>
       </c>
       <c r="L72" t="n">
-        <v>1e-05</v>
+        <v>0.6054726953125001</v>
       </c>
       <c r="M72" t="b">
         <v>1</v>
@@ -5493,7 +5493,7 @@
         <v>0.011</v>
       </c>
       <c r="T72" t="n">
-        <v>-0.056</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="73">
@@ -5517,10 +5517,10 @@
         <v>44.92</v>
       </c>
       <c r="F73" t="n">
-        <v>46.23</v>
+        <v>46.59</v>
       </c>
       <c r="G73" t="n">
-        <v>46.48</v>
+        <v>46.86</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -5535,7 +5535,7 @@
         <v>4</v>
       </c>
       <c r="L73" t="n">
-        <v>1e-05</v>
+        <v>0.6054726953125001</v>
       </c>
       <c r="M73" t="b">
         <v>1</v>
@@ -5563,7 +5563,7 @@
         <v>0.011</v>
       </c>
       <c r="T73" t="n">
-        <v>-0.056</v>
+        <v>-0.061</v>
       </c>
     </row>
     <row r="74">
@@ -5587,10 +5587,10 @@
         <v>50.98</v>
       </c>
       <c r="F74" t="n">
-        <v>45.21</v>
+        <v>45.54</v>
       </c>
       <c r="G74" t="n">
-        <v>45.4</v>
+        <v>46.04</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -5605,7 +5605,7 @@
         <v>0</v>
       </c>
       <c r="L74" t="n">
-        <v>1e-05</v>
+        <v>0.6757844921875001</v>
       </c>
       <c r="M74" t="b">
         <v>1</v>
@@ -5621,19 +5621,19 @@
         </is>
       </c>
       <c r="P74" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q74" t="n">
         <v>0</v>
       </c>
       <c r="R74" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S74" t="n">
         <v>0.011</v>
       </c>
       <c r="T74" t="n">
-        <v>-0.056</v>
+        <v>-0.079</v>
       </c>
     </row>
     <row r="75">
@@ -5657,10 +5657,10 @@
         <v>47.66</v>
       </c>
       <c r="F75" t="n">
-        <v>44.13</v>
+        <v>44.67</v>
       </c>
       <c r="G75" t="n">
-        <v>44.39</v>
+        <v>44.93</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -5675,7 +5675,7 @@
         <v>1</v>
       </c>
       <c r="L75" t="n">
-        <v>1e-05</v>
+        <v>0.6699251757812501</v>
       </c>
       <c r="M75" t="b">
         <v>1</v>
@@ -5691,19 +5691,19 @@
         </is>
       </c>
       <c r="P75" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q75" t="n">
         <v>0</v>
       </c>
       <c r="R75" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S75" t="n">
         <v>0.011</v>
       </c>
       <c r="T75" t="n">
-        <v>-0.057</v>
+        <v>-0.082</v>
       </c>
     </row>
     <row r="76">
@@ -5727,10 +5727,10 @@
         <v>42.08</v>
       </c>
       <c r="F76" t="n">
-        <v>43.14</v>
+        <v>43.67</v>
       </c>
       <c r="G76" t="n">
-        <v>43.37</v>
+        <v>43.93</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -5745,7 +5745,7 @@
         <v>1</v>
       </c>
       <c r="L76" t="n">
-        <v>1e-05</v>
+        <v>0.6562534375000001</v>
       </c>
       <c r="M76" t="b">
         <v>1</v>
@@ -5761,19 +5761,19 @@
         </is>
       </c>
       <c r="P76" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q76" t="n">
         <v>0</v>
       </c>
       <c r="R76" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S76" t="n">
         <v>0.011</v>
       </c>
       <c r="T76" t="n">
-        <v>-0.057</v>
+        <v>-0.083</v>
       </c>
     </row>
     <row r="77">
@@ -5797,10 +5797,10 @@
         <v>41.89</v>
       </c>
       <c r="F77" t="n">
-        <v>42.16</v>
+        <v>42.67</v>
       </c>
       <c r="G77" t="n">
-        <v>42.37</v>
+        <v>42.94</v>
       </c>
       <c r="H77" t="n">
         <v>3.8999977</v>
@@ -5815,7 +5815,7 @@
         <v>17</v>
       </c>
       <c r="L77" t="n">
-        <v>1e-05</v>
+        <v>0.647464462890625</v>
       </c>
       <c r="M77" t="b">
         <v>1</v>
@@ -5831,19 +5831,19 @@
         </is>
       </c>
       <c r="P77" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q77" t="n">
         <v>0</v>
       </c>
       <c r="R77" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S77" t="n">
         <v>0.011</v>
       </c>
       <c r="T77" t="n">
-        <v>-0.057</v>
+        <v>-0.08500000000000001</v>
       </c>
     </row>
     <row r="78">
@@ -5867,10 +5867,10 @@
         <v>44.4</v>
       </c>
       <c r="F78" t="n">
-        <v>41.15</v>
+        <v>41.74</v>
       </c>
       <c r="G78" t="n">
-        <v>41.37</v>
+        <v>42</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -5885,7 +5885,7 @@
         <v>1</v>
       </c>
       <c r="L78" t="n">
-        <v>1e-05</v>
+        <v>0.6777375976562501</v>
       </c>
       <c r="M78" t="b">
         <v>1</v>
@@ -5901,19 +5901,19 @@
         </is>
       </c>
       <c r="P78" t="n">
-        <v>1</v>
+        <v>0.998</v>
       </c>
       <c r="Q78" t="n">
         <v>0</v>
       </c>
       <c r="R78" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="S78" t="n">
         <v>0.011</v>
       </c>
       <c r="T78" t="n">
-        <v>-0.057</v>
+        <v>-0.111</v>
       </c>
     </row>
     <row r="79">
@@ -5937,10 +5937,10 @@
         <v>38.75</v>
       </c>
       <c r="F79" t="n">
-        <v>40.15</v>
+        <v>40.64</v>
       </c>
       <c r="G79" t="n">
-        <v>40.38</v>
+        <v>40.94</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -5955,7 +5955,7 @@
         <v>6</v>
       </c>
       <c r="L79" t="n">
-        <v>1e-05</v>
+        <v>0.6074258007812501</v>
       </c>
       <c r="M79" t="b">
         <v>1</v>
@@ -5971,19 +5971,19 @@
         </is>
       </c>
       <c r="P79" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q79" t="n">
         <v>0</v>
       </c>
       <c r="R79" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S79" t="n">
         <v>0.011</v>
       </c>
       <c r="T79" t="n">
-        <v>-0.057</v>
+        <v>-0.081</v>
       </c>
     </row>
     <row r="80">
@@ -6007,10 +6007,10 @@
         <v>37.95</v>
       </c>
       <c r="F80" t="n">
-        <v>39.13</v>
+        <v>39.56</v>
       </c>
       <c r="G80" t="n">
-        <v>39.37</v>
+        <v>39.81</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -6025,7 +6025,7 @@
         <v>5</v>
       </c>
       <c r="L80" t="n">
-        <v>1e-05</v>
+        <v>0.6093789062500001</v>
       </c>
       <c r="M80" t="b">
         <v>1</v>
@@ -6041,19 +6041,19 @@
         </is>
       </c>
       <c r="P80" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q80" t="n">
         <v>0</v>
       </c>
       <c r="R80" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S80" t="n">
         <v>0.011</v>
       </c>
       <c r="T80" t="n">
-        <v>-0.057</v>
+        <v>-0.08799999999999999</v>
       </c>
     </row>
     <row r="81">
@@ -6077,10 +6077,10 @@
         <v>37.36</v>
       </c>
       <c r="F81" t="n">
-        <v>38.14</v>
+        <v>38.68</v>
       </c>
       <c r="G81" t="n">
-        <v>38.37</v>
+        <v>38.89</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -6095,7 +6095,7 @@
         <v>45</v>
       </c>
       <c r="L81" t="n">
-        <v>1e-05</v>
+        <v>0.57617611328125</v>
       </c>
       <c r="M81" t="b">
         <v>1</v>
@@ -6111,19 +6111,19 @@
         </is>
       </c>
       <c r="P81" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q81" t="n">
         <v>0</v>
       </c>
       <c r="R81" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S81" t="n">
         <v>0.011</v>
       </c>
       <c r="T81" t="n">
-        <v>-0.057</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="82">
@@ -6147,10 +6147,10 @@
         <v>37.43</v>
       </c>
       <c r="F82" t="n">
-        <v>37.15</v>
+        <v>37.46</v>
       </c>
       <c r="G82" t="n">
-        <v>37.4</v>
+        <v>38</v>
       </c>
       <c r="H82" t="n">
         <v>1.0999985</v>
@@ -6165,7 +6165,7 @@
         <v>139</v>
       </c>
       <c r="L82" t="n">
-        <v>1e-05</v>
+        <v>0.5039112109375</v>
       </c>
       <c r="M82" t="b">
         <v>1</v>
@@ -6193,7 +6193,7 @@
         <v>0.011</v>
       </c>
       <c r="T82" t="n">
-        <v>-0.058</v>
+        <v>-0.064</v>
       </c>
     </row>
     <row r="83">
@@ -6217,10 +6217,10 @@
         <v>34.54</v>
       </c>
       <c r="F83" t="n">
-        <v>36.15</v>
+        <v>36.6</v>
       </c>
       <c r="G83" t="n">
-        <v>36.39</v>
+        <v>36.87</v>
       </c>
       <c r="H83" t="n">
         <v>0</v>
@@ -6235,7 +6235,7 @@
         <v>2</v>
       </c>
       <c r="L83" t="n">
-        <v>1e-05</v>
+        <v>0.6054726953125001</v>
       </c>
       <c r="M83" t="b">
         <v>1</v>
@@ -6251,19 +6251,19 @@
         </is>
       </c>
       <c r="P83" t="n">
-        <v>1</v>
+        <v>0.997</v>
       </c>
       <c r="Q83" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R83" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="S83" t="n">
         <v>0.011</v>
       </c>
       <c r="T83" t="n">
-        <v>-0.058</v>
+        <v>-0.115</v>
       </c>
     </row>
     <row r="84">
@@ -6284,28 +6284,28 @@
         <v>402</v>
       </c>
       <c r="E84" t="n">
-        <v>34.82</v>
+        <v>35.7</v>
       </c>
       <c r="F84" t="n">
-        <v>35.18</v>
+        <v>35.57</v>
       </c>
       <c r="G84" t="n">
-        <v>35.41</v>
+        <v>35.81</v>
       </c>
       <c r="H84" t="n">
-        <v>4.029999</v>
+        <v>4.91</v>
       </c>
       <c r="I84" t="n">
-        <v>13.088661</v>
+        <v>15.946735</v>
       </c>
       <c r="J84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K84" t="n">
         <v>5</v>
       </c>
       <c r="L84" t="n">
-        <v>1e-05</v>
+        <v>0.5546919531250001</v>
       </c>
       <c r="M84" t="b">
         <v>1</v>
@@ -6321,19 +6321,19 @@
         </is>
       </c>
       <c r="P84" t="n">
-        <v>1</v>
+        <v>0.998</v>
       </c>
       <c r="Q84" t="n">
         <v>0</v>
       </c>
       <c r="R84" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S84" t="n">
         <v>0.011</v>
       </c>
       <c r="T84" t="n">
-        <v>-0.058</v>
+        <v>-0.091</v>
       </c>
     </row>
     <row r="85">
@@ -6354,28 +6354,28 @@
         <v>403</v>
       </c>
       <c r="E85" t="n">
-        <v>31.88</v>
+        <v>34.76</v>
       </c>
       <c r="F85" t="n">
-        <v>34.22</v>
+        <v>34.68</v>
       </c>
       <c r="G85" t="n">
-        <v>34.43</v>
+        <v>34.94</v>
       </c>
       <c r="H85" t="n">
-        <v>0</v>
+        <v>2.8799992</v>
       </c>
       <c r="I85" t="n">
-        <v>0</v>
+        <v>9.0338745</v>
       </c>
       <c r="J85" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K85" t="n">
         <v>4</v>
       </c>
       <c r="L85" t="n">
-        <v>1e-05</v>
+        <v>0.5400436621093752</v>
       </c>
       <c r="M85" t="b">
         <v>1</v>
@@ -6391,19 +6391,19 @@
         </is>
       </c>
       <c r="P85" t="n">
-        <v>1</v>
+        <v>0.998</v>
       </c>
       <c r="Q85" t="n">
         <v>0</v>
       </c>
       <c r="R85" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S85" t="n">
         <v>0.011</v>
       </c>
       <c r="T85" t="n">
-        <v>-0.058</v>
+        <v>-0.091</v>
       </c>
     </row>
     <row r="86">
@@ -6427,10 +6427,10 @@
         <v>29.31</v>
       </c>
       <c r="F86" t="n">
-        <v>33.22</v>
+        <v>33.6</v>
       </c>
       <c r="G86" t="n">
-        <v>33.43</v>
+        <v>33.87</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -6445,7 +6445,7 @@
         <v>2</v>
       </c>
       <c r="L86" t="n">
-        <v>1e-05</v>
+        <v>0.561527822265625</v>
       </c>
       <c r="M86" t="b">
         <v>1</v>
@@ -6461,19 +6461,19 @@
         </is>
       </c>
       <c r="P86" t="n">
-        <v>1</v>
+        <v>0.997</v>
       </c>
       <c r="Q86" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R86" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="S86" t="n">
         <v>0.011</v>
       </c>
       <c r="T86" t="n">
-        <v>-0.058</v>
+        <v>-0.118</v>
       </c>
     </row>
     <row r="87">
@@ -6497,10 +6497,10 @@
         <v>28.54</v>
       </c>
       <c r="F87" t="n">
-        <v>32.16</v>
+        <v>32.69</v>
       </c>
       <c r="G87" t="n">
-        <v>32.43</v>
+        <v>32.99</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -6515,7 +6515,7 @@
         <v>27</v>
       </c>
       <c r="L87" t="n">
-        <v>1e-05</v>
+        <v>0.5312546875</v>
       </c>
       <c r="M87" t="b">
         <v>1</v>
@@ -6531,19 +6531,19 @@
         </is>
       </c>
       <c r="P87" t="n">
-        <v>1</v>
+        <v>0.998</v>
       </c>
       <c r="Q87" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R87" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="S87" t="n">
         <v>0.011</v>
       </c>
       <c r="T87" t="n">
-        <v>-0.058</v>
+        <v>-0.105</v>
       </c>
     </row>
     <row r="88">
@@ -6567,10 +6567,10 @@
         <v>30.88</v>
       </c>
       <c r="F88" t="n">
-        <v>31.17</v>
+        <v>31.75</v>
       </c>
       <c r="G88" t="n">
-        <v>31.38</v>
+        <v>32.01</v>
       </c>
       <c r="H88" t="n">
         <v>1.3799992</v>
@@ -6585,7 +6585,7 @@
         <v>18</v>
       </c>
       <c r="L88" t="n">
-        <v>1e-05</v>
+        <v>0.5371140039062501</v>
       </c>
       <c r="M88" t="b">
         <v>1</v>
@@ -6601,19 +6601,19 @@
         </is>
       </c>
       <c r="P88" t="n">
-        <v>1</v>
+        <v>0.996</v>
       </c>
       <c r="Q88" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R88" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="S88" t="n">
         <v>0.011</v>
       </c>
       <c r="T88" t="n">
-        <v>-0.058</v>
+        <v>-0.124</v>
       </c>
     </row>
     <row r="89">
@@ -6637,10 +6637,10 @@
         <v>28.72</v>
       </c>
       <c r="F89" t="n">
-        <v>30.14</v>
+        <v>30.58</v>
       </c>
       <c r="G89" t="n">
-        <v>30.38</v>
+        <v>30.82</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -6655,7 +6655,7 @@
         <v>19</v>
       </c>
       <c r="L89" t="n">
-        <v>1e-05</v>
+        <v>0.4902394726562501</v>
       </c>
       <c r="M89" t="b">
         <v>1</v>
@@ -6671,19 +6671,19 @@
         </is>
       </c>
       <c r="P89" t="n">
-        <v>1</v>
+        <v>0.998</v>
       </c>
       <c r="Q89" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R89" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="S89" t="n">
         <v>0.011</v>
       </c>
       <c r="T89" t="n">
-        <v>-0.059</v>
+        <v>-0.097</v>
       </c>
     </row>
     <row r="90">
@@ -6707,10 +6707,10 @@
         <v>27.86</v>
       </c>
       <c r="F90" t="n">
-        <v>29.18</v>
+        <v>29.59</v>
       </c>
       <c r="G90" t="n">
-        <v>29.48</v>
+        <v>30.01</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -6725,7 +6725,7 @@
         <v>32</v>
       </c>
       <c r="L90" t="n">
-        <v>1e-05</v>
+        <v>0.5585981640625001</v>
       </c>
       <c r="M90" t="b">
         <v>1</v>
@@ -6741,19 +6741,19 @@
         </is>
       </c>
       <c r="P90" t="n">
-        <v>1</v>
+        <v>0.992</v>
       </c>
       <c r="Q90" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="R90" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="S90" t="n">
         <v>0.011</v>
       </c>
       <c r="T90" t="n">
-        <v>-0.059</v>
+        <v>-0.195</v>
       </c>
     </row>
     <row r="91">
@@ -6777,10 +6777,10 @@
         <v>27.24</v>
       </c>
       <c r="F91" t="n">
-        <v>28.13</v>
+        <v>28.45</v>
       </c>
       <c r="G91" t="n">
-        <v>28.37</v>
+        <v>29.01</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -6795,7 +6795,7 @@
         <v>11</v>
       </c>
       <c r="L91" t="n">
-        <v>1e-05</v>
+        <v>0.5424850439453126</v>
       </c>
       <c r="M91" t="b">
         <v>1</v>
@@ -6811,19 +6811,19 @@
         </is>
       </c>
       <c r="P91" t="n">
-        <v>1</v>
+        <v>0.992</v>
       </c>
       <c r="Q91" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="R91" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="S91" t="n">
         <v>0.011</v>
       </c>
       <c r="T91" t="n">
-        <v>-0.059</v>
+        <v>-0.196</v>
       </c>
     </row>
     <row r="92">
@@ -6844,28 +6844,28 @@
         <v>410</v>
       </c>
       <c r="E92" t="n">
-        <v>27.44</v>
+        <v>27.45</v>
       </c>
       <c r="F92" t="n">
-        <v>27.19</v>
+        <v>27.63</v>
       </c>
       <c r="G92" t="n">
-        <v>27.42</v>
+        <v>27.87</v>
       </c>
       <c r="H92" t="n">
-        <v>0.32999992</v>
+        <v>0.34000015</v>
       </c>
       <c r="I92" t="n">
-        <v>1.2172627</v>
+        <v>1.2541503</v>
       </c>
       <c r="J92" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K92" t="n">
         <v>3239</v>
       </c>
       <c r="L92" t="n">
-        <v>1e-05</v>
+        <v>0.473638076171875</v>
       </c>
       <c r="M92" t="b">
         <v>1</v>
@@ -6881,19 +6881,19 @@
         </is>
       </c>
       <c r="P92" t="n">
-        <v>1</v>
+        <v>0.996</v>
       </c>
       <c r="Q92" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R92" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="S92" t="n">
         <v>0.011</v>
       </c>
       <c r="T92" t="n">
-        <v>-0.059</v>
+        <v>-0.123</v>
       </c>
     </row>
     <row r="93">
@@ -6917,10 +6917,10 @@
         <v>26.83</v>
       </c>
       <c r="F93" t="n">
-        <v>26.23</v>
+        <v>26.61</v>
       </c>
       <c r="G93" t="n">
-        <v>26.49</v>
+        <v>26.88</v>
       </c>
       <c r="H93" t="n">
         <v>1.2700005</v>
@@ -6935,7 +6935,7 @@
         <v>53</v>
       </c>
       <c r="L93" t="n">
-        <v>1e-05</v>
+        <v>0.46289599609375</v>
       </c>
       <c r="M93" t="b">
         <v>1</v>
@@ -6951,19 +6951,19 @@
         </is>
       </c>
       <c r="P93" t="n">
-        <v>1</v>
+        <v>0.996</v>
       </c>
       <c r="Q93" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R93" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="S93" t="n">
         <v>0.011</v>
       </c>
       <c r="T93" t="n">
-        <v>-0.059</v>
+        <v>-0.129</v>
       </c>
     </row>
     <row r="94">
@@ -6987,10 +6987,10 @@
         <v>25.82</v>
       </c>
       <c r="F94" t="n">
-        <v>25.23</v>
+        <v>25.61</v>
       </c>
       <c r="G94" t="n">
-        <v>25.44</v>
+        <v>25.88</v>
       </c>
       <c r="H94" t="n">
         <v>2.0900002</v>
@@ -7005,7 +7005,7 @@
         <v>15</v>
       </c>
       <c r="L94" t="n">
-        <v>1e-05</v>
+        <v>0.4482477050781249</v>
       </c>
       <c r="M94" t="b">
         <v>1</v>
@@ -7021,19 +7021,19 @@
         </is>
       </c>
       <c r="P94" t="n">
-        <v>1</v>
+        <v>0.995</v>
       </c>
       <c r="Q94" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R94" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="S94" t="n">
         <v>0.011</v>
       </c>
       <c r="T94" t="n">
-        <v>-0.059</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="95">
@@ -7057,10 +7057,10 @@
         <v>24.91</v>
       </c>
       <c r="F95" t="n">
-        <v>24.17</v>
+        <v>24.7</v>
       </c>
       <c r="G95" t="n">
-        <v>24.44</v>
+        <v>24.9</v>
       </c>
       <c r="H95" t="n">
         <v>1.7600002</v>
@@ -7075,7 +7075,7 @@
         <v>10</v>
       </c>
       <c r="L95" t="n">
-        <v>1e-05</v>
+        <v>0.4414118359375</v>
       </c>
       <c r="M95" t="b">
         <v>1</v>
@@ -7091,19 +7091,19 @@
         </is>
       </c>
       <c r="P95" t="n">
-        <v>1</v>
+        <v>0.994</v>
       </c>
       <c r="Q95" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="R95" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="S95" t="n">
         <v>0.011</v>
       </c>
       <c r="T95" t="n">
-        <v>-0.059</v>
+        <v>-0.142</v>
       </c>
     </row>
     <row r="96">
@@ -7127,10 +7127,10 @@
         <v>22.63</v>
       </c>
       <c r="F96" t="n">
-        <v>23.26</v>
+        <v>23.76</v>
       </c>
       <c r="G96" t="n">
-        <v>23.5</v>
+        <v>23.96</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -7145,7 +7145,7 @@
         <v>88</v>
       </c>
       <c r="L96" t="n">
-        <v>1e-05</v>
+        <v>0.44727115234375</v>
       </c>
       <c r="M96" t="b">
         <v>1</v>
@@ -7161,19 +7161,19 @@
         </is>
       </c>
       <c r="P96" t="n">
-        <v>1</v>
+        <v>0.992</v>
       </c>
       <c r="Q96" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="R96" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="S96" t="n">
         <v>0.011</v>
       </c>
       <c r="T96" t="n">
-        <v>-0.06</v>
+        <v>-0.176</v>
       </c>
     </row>
     <row r="97">
@@ -7197,10 +7197,10 @@
         <v>22.4</v>
       </c>
       <c r="F97" t="n">
-        <v>22.25</v>
+        <v>22.7</v>
       </c>
       <c r="G97" t="n">
-        <v>22.48</v>
+        <v>22.91</v>
       </c>
       <c r="H97" t="n">
         <v>0.4300003</v>
@@ -7215,7 +7215,7 @@
         <v>568</v>
       </c>
       <c r="L97" t="n">
-        <v>1e-05</v>
+        <v>0.4145566357421875</v>
       </c>
       <c r="M97" t="b">
         <v>1</v>
@@ -7231,19 +7231,19 @@
         </is>
       </c>
       <c r="P97" t="n">
-        <v>1</v>
+        <v>0.993</v>
       </c>
       <c r="Q97" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="R97" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="S97" t="n">
         <v>0.011</v>
       </c>
       <c r="T97" t="n">
-        <v>-0.06</v>
+        <v>-0.149</v>
       </c>
     </row>
     <row r="98">
@@ -7267,10 +7267,10 @@
         <v>21.15</v>
       </c>
       <c r="F98" t="n">
-        <v>21.23</v>
+        <v>21.6</v>
       </c>
       <c r="G98" t="n">
-        <v>21.46</v>
+        <v>21.83</v>
       </c>
       <c r="H98" t="n">
         <v>2.959999</v>
@@ -7285,7 +7285,7 @@
         <v>121</v>
       </c>
       <c r="L98" t="n">
-        <v>1e-05</v>
+        <v>0.368170380859375</v>
       </c>
       <c r="M98" t="b">
         <v>1</v>
@@ -7301,19 +7301,19 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>1</v>
+        <v>0.996</v>
       </c>
       <c r="Q98" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R98" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="S98" t="n">
         <v>0.011</v>
       </c>
       <c r="T98" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="99">
@@ -7337,10 +7337,10 @@
         <v>19.15</v>
       </c>
       <c r="F99" t="n">
-        <v>20.17</v>
+        <v>20.64</v>
       </c>
       <c r="G99" t="n">
-        <v>20.41</v>
+        <v>20.88</v>
       </c>
       <c r="H99" t="n">
         <v>1.1399994</v>
@@ -7355,7 +7355,7 @@
         <v>22</v>
       </c>
       <c r="L99" t="n">
-        <v>1e-05</v>
+        <v>0.37305314453125</v>
       </c>
       <c r="M99" t="b">
         <v>1</v>
@@ -7371,19 +7371,19 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>1</v>
+        <v>0.994</v>
       </c>
       <c r="Q99" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="R99" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="S99" t="n">
         <v>0.011</v>
       </c>
       <c r="T99" t="n">
-        <v>-0.06</v>
+        <v>-0.136</v>
       </c>
     </row>
     <row r="100">
@@ -7407,10 +7407,10 @@
         <v>17.95</v>
       </c>
       <c r="F100" t="n">
-        <v>19.17</v>
+        <v>19.7</v>
       </c>
       <c r="G100" t="n">
-        <v>19.39</v>
+        <v>19.96</v>
       </c>
       <c r="H100" t="n">
         <v>0</v>
@@ -7425,7 +7425,7 @@
         <v>46</v>
       </c>
       <c r="L100" t="n">
-        <v>1e-05</v>
+        <v>0.383795224609375</v>
       </c>
       <c r="M100" t="b">
         <v>1</v>
@@ -7441,19 +7441,19 @@
         </is>
       </c>
       <c r="P100" t="n">
-        <v>1</v>
+        <v>0.989</v>
       </c>
       <c r="Q100" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="R100" t="n">
-        <v>0</v>
+        <v>0.006</v>
       </c>
       <c r="S100" t="n">
         <v>0.011</v>
       </c>
       <c r="T100" t="n">
-        <v>-0.06</v>
+        <v>-0.182</v>
       </c>
     </row>
     <row r="101">
@@ -7477,10 +7477,10 @@
         <v>14.74</v>
       </c>
       <c r="F101" t="n">
-        <v>18.18</v>
+        <v>18.6</v>
       </c>
       <c r="G101" t="n">
-        <v>18.45</v>
+        <v>18.84</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
@@ -7495,7 +7495,7 @@
         <v>54</v>
       </c>
       <c r="L101" t="n">
-        <v>1e-05</v>
+        <v>0.32813171875</v>
       </c>
       <c r="M101" t="b">
         <v>1</v>
@@ -7511,19 +7511,19 @@
         </is>
       </c>
       <c r="P101" t="n">
-        <v>1</v>
+        <v>0.995</v>
       </c>
       <c r="Q101" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="R101" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="S101" t="n">
         <v>0.011</v>
       </c>
       <c r="T101" t="n">
-        <v>-0.06</v>
+        <v>-0.117</v>
       </c>
     </row>
     <row r="102">
@@ -7544,28 +7544,28 @@
         <v>420</v>
       </c>
       <c r="E102" t="n">
-        <v>17.57</v>
+        <v>17.5</v>
       </c>
       <c r="F102" t="n">
-        <v>17.14</v>
+        <v>17.62</v>
       </c>
       <c r="G102" t="n">
-        <v>17.37</v>
+        <v>17.89</v>
       </c>
       <c r="H102" t="n">
-        <v>1.7599993</v>
+        <v>1.6899996</v>
       </c>
       <c r="I102" t="n">
-        <v>11.13219</v>
+        <v>10.689434</v>
       </c>
       <c r="J102" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K102" t="n">
         <v>5924</v>
       </c>
       <c r="L102" t="n">
-        <v>1e-05</v>
+        <v>0.331061376953125</v>
       </c>
       <c r="M102" t="b">
         <v>1</v>
@@ -7581,19 +7581,19 @@
         </is>
       </c>
       <c r="P102" t="n">
-        <v>1</v>
+        <v>0.992</v>
       </c>
       <c r="Q102" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="R102" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="S102" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T102" t="n">
-        <v>-0.06</v>
+        <v>-0.146</v>
       </c>
     </row>
     <row r="103">
@@ -7617,10 +7617,10 @@
         <v>17.3</v>
       </c>
       <c r="F103" t="n">
-        <v>16.24</v>
+        <v>16.64</v>
       </c>
       <c r="G103" t="n">
-        <v>16.5</v>
+        <v>17.03</v>
       </c>
       <c r="H103" t="n">
         <v>2.8099995</v>
@@ -7635,7 +7635,7 @@
         <v>116</v>
       </c>
       <c r="L103" t="n">
-        <v>1e-05</v>
+        <v>0.3535220898437499</v>
       </c>
       <c r="M103" t="b">
         <v>1</v>
@@ -7651,19 +7651,19 @@
         </is>
       </c>
       <c r="P103" t="n">
-        <v>1</v>
+        <v>0.983</v>
       </c>
       <c r="Q103" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="R103" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="S103" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T103" t="n">
-        <v>-0.061</v>
+        <v>-0.232</v>
       </c>
     </row>
     <row r="104">
@@ -7687,10 +7687,10 @@
         <v>14.82</v>
       </c>
       <c r="F104" t="n">
-        <v>15.17</v>
+        <v>15.59</v>
       </c>
       <c r="G104" t="n">
-        <v>15.43</v>
+        <v>15.84</v>
       </c>
       <c r="H104" t="n">
         <v>0.5799999</v>
@@ -7705,7 +7705,7 @@
         <v>105</v>
       </c>
       <c r="L104" t="n">
-        <v>1e-05</v>
+        <v>0.2832102929687499</v>
       </c>
       <c r="M104" t="b">
         <v>1</v>
@@ -7721,19 +7721,19 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>1</v>
+        <v>0.993</v>
       </c>
       <c r="Q104" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="R104" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="S104" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T104" t="n">
-        <v>-0.061</v>
+        <v>-0.121</v>
       </c>
     </row>
     <row r="105">
@@ -7754,28 +7754,28 @@
         <v>423</v>
       </c>
       <c r="E105" t="n">
+        <v>14.67</v>
+      </c>
+      <c r="F105" t="n">
+        <v>14.61</v>
+      </c>
+      <c r="G105" t="n">
         <v>14.84</v>
       </c>
-      <c r="F105" t="n">
-        <v>14.2</v>
-      </c>
-      <c r="G105" t="n">
-        <v>14.44</v>
-      </c>
       <c r="H105" t="n">
-        <v>0.8400001499999999</v>
+        <v>0.6700001</v>
       </c>
       <c r="I105" t="n">
-        <v>6.000001</v>
+        <v>4.7857146</v>
       </c>
       <c r="J105" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K105" t="n">
         <v>293</v>
       </c>
       <c r="L105" t="n">
-        <v>1e-05</v>
+        <v>0.268562001953125</v>
       </c>
       <c r="M105" t="b">
         <v>1</v>
@@ -7791,19 +7791,19 @@
         </is>
       </c>
       <c r="P105" t="n">
-        <v>1</v>
+        <v>0.993</v>
       </c>
       <c r="Q105" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="R105" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="S105" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T105" t="n">
-        <v>-0.061</v>
+        <v>-0.123</v>
       </c>
     </row>
     <row r="106">
@@ -7824,28 +7824,28 @@
         <v>424</v>
       </c>
       <c r="E106" t="n">
-        <v>13.2</v>
+        <v>13.7</v>
       </c>
       <c r="F106" t="n">
-        <v>13.21</v>
+        <v>13.72</v>
       </c>
       <c r="G106" t="n">
-        <v>13.46</v>
+        <v>13.97</v>
       </c>
       <c r="H106" t="n">
-        <v>1.3199997</v>
+        <v>1.8199997</v>
       </c>
       <c r="I106" t="n">
-        <v>11.111109</v>
+        <v>15.319862</v>
       </c>
       <c r="J106" t="n">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="K106" t="n">
         <v>723</v>
       </c>
       <c r="L106" t="n">
-        <v>1e-05</v>
+        <v>0.2890696093749999</v>
       </c>
       <c r="M106" t="b">
         <v>1</v>
@@ -7861,19 +7861,19 @@
         </is>
       </c>
       <c r="P106" t="n">
-        <v>1</v>
+        <v>0.983</v>
       </c>
       <c r="Q106" t="n">
-        <v>0</v>
+        <v>0.006</v>
       </c>
       <c r="R106" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="S106" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T106" t="n">
-        <v>-0.061</v>
+        <v>-0.201</v>
       </c>
     </row>
     <row r="107">
@@ -7894,28 +7894,28 @@
         <v>425</v>
       </c>
       <c r="E107" t="n">
-        <v>12.29</v>
+        <v>12.7</v>
       </c>
       <c r="F107" t="n">
-        <v>12.17</v>
+        <v>12.52</v>
       </c>
       <c r="G107" t="n">
-        <v>12.46</v>
+        <v>13.03</v>
       </c>
       <c r="H107" t="n">
-        <v>1.4399996</v>
+        <v>1.8499994</v>
       </c>
       <c r="I107" t="n">
-        <v>13.271885</v>
+        <v>17.050686</v>
       </c>
       <c r="J107" t="n">
-        <v>773</v>
+        <v>780</v>
       </c>
       <c r="K107" t="n">
         <v>1152</v>
       </c>
       <c r="L107" t="n">
-        <v>1e-05</v>
+        <v>0.2856516748046874</v>
       </c>
       <c r="M107" t="b">
         <v>1</v>
@@ -7931,19 +7931,19 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>1</v>
+        <v>0.976</v>
       </c>
       <c r="Q107" t="n">
-        <v>0</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="R107" t="n">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="S107" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T107" t="n">
-        <v>-0.061</v>
+        <v>-0.243</v>
       </c>
     </row>
     <row r="108">
@@ -7964,28 +7964,28 @@
         <v>426</v>
       </c>
       <c r="E108" t="n">
-        <v>11.36</v>
+        <v>11.67</v>
       </c>
       <c r="F108" t="n">
-        <v>11.2</v>
+        <v>11.5</v>
       </c>
       <c r="G108" t="n">
-        <v>11.44</v>
+        <v>12.04</v>
       </c>
       <c r="H108" t="n">
-        <v>1.1899996</v>
+        <v>1.5</v>
       </c>
       <c r="I108" t="n">
-        <v>11.701077</v>
+        <v>14.749263</v>
       </c>
       <c r="J108" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K108" t="n">
         <v>1952</v>
       </c>
       <c r="L108" t="n">
-        <v>1e-05</v>
+        <v>0.2700268310546875</v>
       </c>
       <c r="M108" t="b">
         <v>1</v>
@@ -8001,19 +8001,19 @@
         </is>
       </c>
       <c r="P108" t="n">
-        <v>1</v>
+        <v>0.973</v>
       </c>
       <c r="Q108" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="R108" t="n">
-        <v>0</v>
+        <v>0.014</v>
       </c>
       <c r="S108" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T108" t="n">
-        <v>-0.061</v>
+        <v>-0.252</v>
       </c>
     </row>
     <row r="109">
@@ -8034,28 +8034,28 @@
         <v>427</v>
       </c>
       <c r="E109" t="n">
-        <v>10.11</v>
+        <v>10.92</v>
       </c>
       <c r="F109" t="n">
-        <v>10.21</v>
+        <v>10.79</v>
       </c>
       <c r="G109" t="n">
-        <v>10.4</v>
+        <v>10.91</v>
       </c>
       <c r="H109" t="n">
-        <v>0.069999695</v>
+        <v>0.8800001</v>
       </c>
       <c r="I109" t="n">
-        <v>0.6972081</v>
+        <v>8.764942</v>
       </c>
       <c r="J109" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="K109" t="n">
         <v>2220</v>
       </c>
       <c r="L109" t="n">
-        <v>1e-05</v>
+        <v>0.2251054052734375</v>
       </c>
       <c r="M109" t="b">
         <v>1</v>
@@ -8071,19 +8071,19 @@
         </is>
       </c>
       <c r="P109" t="n">
-        <v>1</v>
+        <v>0.983</v>
       </c>
       <c r="Q109" t="n">
-        <v>0</v>
+        <v>0.008</v>
       </c>
       <c r="R109" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="S109" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T109" t="n">
-        <v>-0.061</v>
+        <v>-0.171</v>
       </c>
     </row>
     <row r="110">
@@ -8104,28 +8104,28 @@
         <v>428</v>
       </c>
       <c r="E110" t="n">
-        <v>9.300000000000001</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="F110" t="n">
-        <v>9.19</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="G110" t="n">
-        <v>9.43</v>
+        <v>9.94</v>
       </c>
       <c r="H110" t="n">
-        <v>0.6500006</v>
+        <v>1.0500002</v>
       </c>
       <c r="I110" t="n">
-        <v>7.514458</v>
+        <v>12.138731</v>
       </c>
       <c r="J110" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K110" t="n">
         <v>2784</v>
       </c>
       <c r="L110" t="n">
-        <v>1e-05</v>
+        <v>0.2153398779296875</v>
       </c>
       <c r="M110" t="b">
         <v>1</v>
@@ -8141,19 +8141,19 @@
         </is>
       </c>
       <c r="P110" t="n">
-        <v>1</v>
+        <v>0.977</v>
       </c>
       <c r="Q110" t="n">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="R110" t="n">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="S110" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T110" t="n">
-        <v>-0.062</v>
+        <v>-0.193</v>
       </c>
     </row>
     <row r="111">
@@ -8174,28 +8174,28 @@
         <v>429</v>
       </c>
       <c r="E111" t="n">
-        <v>8.34</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="F111" t="n">
-        <v>8.23</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="G111" t="n">
-        <v>8.44</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="H111" t="n">
-        <v>0.34000015</v>
+        <v>0.77999973</v>
       </c>
       <c r="I111" t="n">
-        <v>4.250002</v>
+        <v>9.749995999999999</v>
       </c>
       <c r="J111" t="n">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="K111" t="n">
         <v>2052</v>
       </c>
       <c r="L111" t="n">
-        <v>1e-05</v>
+        <v>0.2182695361328125</v>
       </c>
       <c r="M111" t="b">
         <v>1</v>
@@ -8211,19 +8211,19 @@
         </is>
       </c>
       <c r="P111" t="n">
-        <v>1</v>
+        <v>0.962</v>
       </c>
       <c r="Q111" t="n">
-        <v>0</v>
+        <v>0.017</v>
       </c>
       <c r="R111" t="n">
-        <v>0</v>
+        <v>0.019</v>
       </c>
       <c r="S111" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T111" t="n">
-        <v>-0.062</v>
+        <v>-0.268</v>
       </c>
     </row>
     <row r="112">
@@ -8244,28 +8244,28 @@
         <v>430</v>
       </c>
       <c r="E112" t="n">
-        <v>7.35</v>
+        <v>7.81</v>
       </c>
       <c r="F112" t="n">
-        <v>7.23</v>
+        <v>7.61</v>
       </c>
       <c r="G112" t="n">
-        <v>7.49</v>
+        <v>7.85</v>
       </c>
       <c r="H112" t="n">
-        <v>0.3499999</v>
+        <v>0.80999994</v>
       </c>
       <c r="I112" t="n">
-        <v>4.999999</v>
+        <v>11.571427</v>
       </c>
       <c r="J112" t="n">
-        <v>2622</v>
+        <v>2660</v>
       </c>
       <c r="K112" t="n">
         <v>30216</v>
       </c>
       <c r="L112" t="n">
-        <v>1e-05</v>
+        <v>0.16211775390625</v>
       </c>
       <c r="M112" t="b">
         <v>1</v>
@@ -8281,19 +8281,19 @@
         </is>
       </c>
       <c r="P112" t="n">
-        <v>1</v>
+        <v>0.982</v>
       </c>
       <c r="Q112" t="n">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="R112" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="S112" t="n">
         <v>0.012</v>
       </c>
       <c r="T112" t="n">
-        <v>-0.062</v>
+        <v>-0.142</v>
       </c>
     </row>
     <row r="113">
@@ -8314,28 +8314,28 @@
         <v>431</v>
       </c>
       <c r="E113" t="n">
-        <v>6.34</v>
+        <v>6.75</v>
       </c>
       <c r="F113" t="n">
-        <v>6.32</v>
+        <v>6.83</v>
       </c>
       <c r="G113" t="n">
-        <v>6.49</v>
+        <v>7</v>
       </c>
       <c r="H113" t="n">
-        <v>0.21000004</v>
+        <v>0.6199999</v>
       </c>
       <c r="I113" t="n">
-        <v>3.4257755</v>
+        <v>10.11419</v>
       </c>
       <c r="J113" t="n">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="K113" t="n">
         <v>2101</v>
       </c>
       <c r="L113" t="n">
-        <v>1e-05</v>
+        <v>0.172859833984375</v>
       </c>
       <c r="M113" t="b">
         <v>1</v>
@@ -8351,19 +8351,19 @@
         </is>
       </c>
       <c r="P113" t="n">
-        <v>1</v>
+        <v>0.957</v>
       </c>
       <c r="Q113" t="n">
-        <v>0</v>
+        <v>0.023</v>
       </c>
       <c r="R113" t="n">
-        <v>0</v>
+        <v>0.021</v>
       </c>
       <c r="S113" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T113" t="n">
-        <v>-0.062</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="114">
@@ -8384,28 +8384,28 @@
         <v>432</v>
       </c>
       <c r="E114" t="n">
-        <v>5.5</v>
+        <v>5.94</v>
       </c>
       <c r="F114" t="n">
-        <v>5.37</v>
+        <v>5.58</v>
       </c>
       <c r="G114" t="n">
-        <v>5.55</v>
+        <v>6</v>
       </c>
       <c r="H114" t="n">
-        <v>0.26000023</v>
+        <v>0.7000003</v>
       </c>
       <c r="I114" t="n">
-        <v>4.961837</v>
+        <v>13.358786</v>
       </c>
       <c r="J114" t="n">
-        <v>1026</v>
+        <v>1071</v>
       </c>
       <c r="K114" t="n">
         <v>6856</v>
       </c>
       <c r="L114" t="n">
-        <v>0.09180595703125</v>
+        <v>0.1540611938476563</v>
       </c>
       <c r="M114" t="b">
         <v>1</v>
@@ -8421,19 +8421,19 @@
         </is>
       </c>
       <c r="P114" t="n">
-        <v>0.996</v>
+        <v>0.949</v>
       </c>
       <c r="Q114" t="n">
-        <v>0.005</v>
+        <v>0.03</v>
       </c>
       <c r="R114" t="n">
-        <v>0.003</v>
+        <v>0.024</v>
       </c>
       <c r="S114" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T114" t="n">
-        <v>-0.074</v>
+        <v>-0.243</v>
       </c>
     </row>
     <row r="115">
@@ -8454,28 +8454,28 @@
         <v>433</v>
       </c>
       <c r="E115" t="n">
-        <v>4.5</v>
+        <v>4.9</v>
       </c>
       <c r="F115" t="n">
-        <v>4.38</v>
+        <v>4.71</v>
       </c>
       <c r="G115" t="n">
-        <v>4.54</v>
+        <v>4.99</v>
       </c>
       <c r="H115" t="n">
-        <v>0.119999886</v>
+        <v>0.52</v>
       </c>
       <c r="I115" t="n">
-        <v>2.7397234</v>
+        <v>11.872146</v>
       </c>
       <c r="J115" t="n">
-        <v>1490</v>
+        <v>1533</v>
       </c>
       <c r="K115" t="n">
         <v>13287</v>
       </c>
       <c r="L115" t="n">
-        <v>0.073251455078125</v>
+        <v>0.1333094482421875</v>
       </c>
       <c r="M115" t="b">
         <v>1</v>
@@ -8491,19 +8491,19 @@
         </is>
       </c>
       <c r="P115" t="n">
-        <v>0.997</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="Q115" t="n">
-        <v>0.005</v>
+        <v>0.039</v>
       </c>
       <c r="R115" t="n">
-        <v>0.002</v>
+        <v>0.027</v>
       </c>
       <c r="S115" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T115" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-0.239</v>
       </c>
     </row>
     <row r="116">
@@ -8524,28 +8524,28 @@
         <v>434</v>
       </c>
       <c r="E116" t="n">
-        <v>3.62</v>
+        <v>4</v>
       </c>
       <c r="F116" t="n">
-        <v>3.53</v>
+        <v>3.9</v>
       </c>
       <c r="G116" t="n">
-        <v>3.67</v>
+        <v>4.1</v>
       </c>
       <c r="H116" t="n">
-        <v>-0.010000229</v>
+        <v>0.3699999</v>
       </c>
       <c r="I116" t="n">
-        <v>-0.27548838</v>
+        <v>10.192834</v>
       </c>
       <c r="J116" t="n">
-        <v>4671</v>
+        <v>4838</v>
       </c>
       <c r="K116" t="n">
         <v>19106</v>
       </c>
       <c r="L116" t="n">
-        <v>0.0893645751953125</v>
+        <v>0.12696185546875</v>
       </c>
       <c r="M116" t="b">
         <v>1</v>
@@ -8561,19 +8561,19 @@
         </is>
       </c>
       <c r="P116" t="n">
-        <v>0.961</v>
+        <v>0.902</v>
       </c>
       <c r="Q116" t="n">
-        <v>0.041</v>
+        <v>0.06</v>
       </c>
       <c r="R116" t="n">
-        <v>0.019</v>
+        <v>0.04</v>
       </c>
       <c r="S116" t="n">
         <v>0.011</v>
       </c>
       <c r="T116" t="n">
-        <v>-0.147</v>
+        <v>-0.309</v>
       </c>
     </row>
     <row r="117">
@@ -8594,28 +8594,28 @@
         <v>435</v>
       </c>
       <c r="E117" t="n">
-        <v>2.77</v>
+        <v>3.29</v>
       </c>
       <c r="F117" t="n">
-        <v>2.8</v>
+        <v>3.22</v>
       </c>
       <c r="G117" t="n">
-        <v>2.82</v>
+        <v>3.29</v>
       </c>
       <c r="H117" t="n">
-        <v>-0.1500001</v>
+        <v>0.3699999</v>
       </c>
       <c r="I117" t="n">
-        <v>-5.1369896</v>
+        <v>12.671228</v>
       </c>
       <c r="J117" t="n">
-        <v>30143</v>
+        <v>30393</v>
       </c>
       <c r="K117" t="n">
         <v>30201</v>
       </c>
       <c r="L117" t="n">
-        <v>0.0893645751953125</v>
+        <v>0.124032197265625</v>
       </c>
       <c r="M117" t="b">
         <v>1</v>
@@ -8631,19 +8631,19 @@
         </is>
       </c>
       <c r="P117" t="n">
-        <v>0.898</v>
+        <v>0.833</v>
       </c>
       <c r="Q117" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="R117" t="n">
-        <v>0.041</v>
+        <v>0.057</v>
       </c>
       <c r="S117" t="n">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="T117" t="n">
-        <v>-0.239</v>
+        <v>-0.407</v>
       </c>
     </row>
     <row r="118">
@@ -8664,28 +8664,28 @@
         <v>436</v>
       </c>
       <c r="E118" t="n">
-        <v>2.14</v>
+        <v>2.37</v>
       </c>
       <c r="F118" t="n">
-        <v>2.1</v>
+        <v>2.49</v>
       </c>
       <c r="G118" t="n">
-        <v>2.11</v>
+        <v>2.52</v>
       </c>
       <c r="H118" t="n">
-        <v>-0.119999886</v>
+        <v>0.109999895</v>
       </c>
       <c r="I118" t="n">
-        <v>-5.3097296</v>
+        <v>4.867252</v>
       </c>
       <c r="J118" t="n">
-        <v>66970</v>
+        <v>68847</v>
       </c>
       <c r="K118" t="n">
         <v>18735</v>
       </c>
       <c r="L118" t="n">
-        <v>0.09327078613281251</v>
+        <v>0.1184170190429688</v>
       </c>
       <c r="M118" t="b">
         <v>1</v>
@@ -8701,19 +8701,19 @@
         </is>
       </c>
       <c r="P118" t="n">
-        <v>0.772</v>
+        <v>0.739</v>
       </c>
       <c r="Q118" t="n">
-        <v>0.142</v>
+        <v>0.12</v>
       </c>
       <c r="R118" t="n">
-        <v>0.06900000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="S118" t="n">
         <v>0.008999999999999999</v>
       </c>
       <c r="T118" t="n">
-        <v>-0.371</v>
+        <v>-0.487</v>
       </c>
     </row>
     <row r="119">
@@ -8734,28 +8734,28 @@
         <v>437</v>
       </c>
       <c r="E119" t="n">
-        <v>1.54</v>
+        <v>1.71</v>
       </c>
       <c r="F119" t="n">
-        <v>1.48</v>
+        <v>1.79</v>
       </c>
       <c r="G119" t="n">
-        <v>1.49</v>
+        <v>1.8</v>
       </c>
       <c r="H119" t="n">
-        <v>-0.1500001</v>
+        <v>0.01999998</v>
       </c>
       <c r="I119" t="n">
-        <v>-8.875745</v>
+        <v>1.1834308</v>
       </c>
       <c r="J119" t="n">
-        <v>143392</v>
+        <v>150147</v>
       </c>
       <c r="K119" t="n">
         <v>17089</v>
       </c>
       <c r="L119" t="n">
-        <v>0.09412526977539062</v>
+        <v>0.1106045971679687</v>
       </c>
       <c r="M119" t="b">
         <v>1</v>
@@ -8771,10 +8771,10 @@
         </is>
       </c>
       <c r="P119" t="n">
-        <v>0.608</v>
+        <v>0.614</v>
       </c>
       <c r="Q119" t="n">
-        <v>0.178</v>
+        <v>0.151</v>
       </c>
       <c r="R119" t="n">
         <v>0.08799999999999999</v>
@@ -8783,7 +8783,7 @@
         <v>0.007</v>
       </c>
       <c r="T119" t="n">
-        <v>-0.452</v>
+        <v>-0.523</v>
       </c>
     </row>
     <row r="120">
@@ -8804,28 +8804,28 @@
         <v>438</v>
       </c>
       <c r="E120" t="n">
-        <v>1.04</v>
+        <v>1.2</v>
       </c>
       <c r="F120" t="n">
-        <v>1.04</v>
+        <v>1.17</v>
       </c>
       <c r="G120" t="n">
-        <v>1.05</v>
+        <v>1.18</v>
       </c>
       <c r="H120" t="n">
-        <v>-0.19000006</v>
+        <v>-0.029999971</v>
       </c>
       <c r="I120" t="n">
-        <v>-15.447159</v>
+        <v>-2.439022</v>
       </c>
       <c r="J120" t="n">
-        <v>167479</v>
+        <v>179470</v>
       </c>
       <c r="K120" t="n">
         <v>21427</v>
       </c>
       <c r="L120" t="n">
-        <v>0.09888596435546876</v>
+        <v>0.1027921752929687</v>
       </c>
       <c r="M120" t="b">
         <v>0</v>
@@ -8841,19 +8841,19 @@
         </is>
       </c>
       <c r="P120" t="n">
-        <v>0.428</v>
+        <v>0.455</v>
       </c>
       <c r="Q120" t="n">
-        <v>0.173</v>
+        <v>0.168</v>
       </c>
       <c r="R120" t="n">
-        <v>0.09</v>
+        <v>0.091</v>
       </c>
       <c r="S120" t="n">
         <v>0.005</v>
       </c>
       <c r="T120" t="n">
-        <v>-0.471</v>
+        <v>-0.495</v>
       </c>
     </row>
     <row r="121">
@@ -8874,28 +8874,28 @@
         <v>439</v>
       </c>
       <c r="E121" t="n">
-        <v>0.66</v>
+        <v>0.76</v>
       </c>
       <c r="F121" t="n">
-        <v>0.64</v>
+        <v>0.82</v>
       </c>
       <c r="G121" t="n">
-        <v>0.65</v>
+        <v>0.83</v>
       </c>
       <c r="H121" t="n">
-        <v>-0.19</v>
+        <v>-0.09000002999999999</v>
       </c>
       <c r="I121" t="n">
-        <v>-22.35294</v>
+        <v>-10.588239</v>
       </c>
       <c r="J121" t="n">
-        <v>71417</v>
+        <v>74884</v>
       </c>
       <c r="K121" t="n">
         <v>16838</v>
       </c>
       <c r="L121" t="n">
-        <v>0.09693285888671876</v>
+        <v>0.1071866625976562</v>
       </c>
       <c r="M121" t="b">
         <v>0</v>
@@ -8911,19 +8911,19 @@
         </is>
       </c>
       <c r="P121" t="n">
-        <v>0.263</v>
+        <v>0.303</v>
       </c>
       <c r="Q121" t="n">
-        <v>0.147</v>
+        <v>0.142</v>
       </c>
       <c r="R121" t="n">
-        <v>0.075</v>
+        <v>0.08</v>
       </c>
       <c r="S121" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="T121" t="n">
-        <v>-0.379</v>
+        <v>-0.448</v>
       </c>
     </row>
     <row r="122">
@@ -8944,28 +8944,28 @@
         <v>440</v>
       </c>
       <c r="E122" t="n">
-        <v>0.42</v>
+        <v>0.49</v>
       </c>
       <c r="F122" t="n">
-        <v>0.41</v>
+        <v>0.51</v>
       </c>
       <c r="G122" t="n">
-        <v>0.42</v>
+        <v>0.52</v>
       </c>
       <c r="H122" t="n">
-        <v>-0.15</v>
+        <v>-0.07999998</v>
       </c>
       <c r="I122" t="n">
-        <v>-26.31579</v>
+        <v>-14.035085</v>
       </c>
       <c r="J122" t="n">
-        <v>87395</v>
+        <v>89737</v>
       </c>
       <c r="K122" t="n">
         <v>38206</v>
       </c>
       <c r="L122" t="n">
-        <v>0.100594931640625</v>
+        <v>0.1063321789550781</v>
       </c>
       <c r="M122" t="b">
         <v>0</v>
@@ -8981,19 +8981,19 @@
         </is>
       </c>
       <c r="P122" t="n">
-        <v>0.148</v>
+        <v>0.177</v>
       </c>
       <c r="Q122" t="n">
-        <v>0.1</v>
+        <v>0.107</v>
       </c>
       <c r="R122" t="n">
-        <v>0.053</v>
+        <v>0.059</v>
       </c>
       <c r="S122" t="n">
         <v>0.002</v>
       </c>
       <c r="T122" t="n">
-        <v>-0.276</v>
+        <v>-0.327</v>
       </c>
     </row>
     <row r="123">
@@ -9014,28 +9014,28 @@
         <v>441</v>
       </c>
       <c r="E123" t="n">
-        <v>0.25</v>
+        <v>0.29</v>
       </c>
       <c r="F123" t="n">
-        <v>0.24</v>
+        <v>0.31</v>
       </c>
       <c r="G123" t="n">
-        <v>0.25</v>
+        <v>0.32</v>
       </c>
       <c r="H123" t="n">
-        <v>-0.120000005</v>
+        <v>-0.08000001</v>
       </c>
       <c r="I123" t="n">
-        <v>-32.432434</v>
+        <v>-21.621626</v>
       </c>
       <c r="J123" t="n">
-        <v>31504</v>
+        <v>33461</v>
       </c>
       <c r="K123" t="n">
         <v>13128</v>
       </c>
       <c r="L123" t="n">
-        <v>0.1018156225585937</v>
+        <v>0.1071866625976562</v>
       </c>
       <c r="M123" t="b">
         <v>0</v>
@@ -9051,19 +9051,19 @@
         </is>
       </c>
       <c r="P123" t="n">
-        <v>0.073</v>
+        <v>0.093</v>
       </c>
       <c r="Q123" t="n">
-        <v>0.059</v>
+        <v>0.068</v>
       </c>
       <c r="R123" t="n">
-        <v>0.032</v>
+        <v>0.038</v>
       </c>
       <c r="S123" t="n">
         <v>0.001</v>
       </c>
       <c r="T123" t="n">
-        <v>-0.165</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="124">
@@ -9084,28 +9084,28 @@
         <v>442</v>
       </c>
       <c r="E124" t="n">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="F124" t="n">
-        <v>0.14</v>
+        <v>0.17</v>
       </c>
       <c r="G124" t="n">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="H124" t="n">
-        <v>-0.06999999</v>
+        <v>-0.030000001</v>
       </c>
       <c r="I124" t="n">
-        <v>-31.818178</v>
+        <v>-13.636364</v>
       </c>
       <c r="J124" t="n">
-        <v>32294</v>
+        <v>32915</v>
       </c>
       <c r="K124" t="n">
         <v>36827</v>
       </c>
       <c r="L124" t="n">
-        <v>0.1047452807617187</v>
+        <v>0.1069425244140625</v>
       </c>
       <c r="M124" t="b">
         <v>0</v>
@@ -9121,19 +9121,19 @@
         </is>
       </c>
       <c r="P124" t="n">
-        <v>0.034</v>
+        <v>0.042</v>
       </c>
       <c r="Q124" t="n">
-        <v>0.031</v>
+        <v>0.036</v>
       </c>
       <c r="R124" t="n">
-        <v>0.017</v>
+        <v>0.02</v>
       </c>
       <c r="S124" t="n">
         <v>0</v>
       </c>
       <c r="T124" t="n">
-        <v>-0.092</v>
+        <v>-0.112</v>
       </c>
     </row>
     <row r="125">
@@ -9154,28 +9154,28 @@
         <v>443</v>
       </c>
       <c r="E125" t="n">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="F125" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="G125" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="H125" t="n">
-        <v>-0.060000002</v>
+        <v>-0.030000001</v>
       </c>
       <c r="I125" t="n">
-        <v>-42.857143</v>
+        <v>-21.428572</v>
       </c>
       <c r="J125" t="n">
-        <v>13143</v>
+        <v>14102</v>
       </c>
       <c r="K125" t="n">
         <v>7898</v>
       </c>
       <c r="L125" t="n">
-        <v>0.1079190771484375</v>
+        <v>0.1098721826171875</v>
       </c>
       <c r="M125" t="b">
         <v>0</v>
@@ -9191,19 +9191,19 @@
         </is>
       </c>
       <c r="P125" t="n">
-        <v>0.015</v>
+        <v>0.019</v>
       </c>
       <c r="Q125" t="n">
-        <v>0.015</v>
+        <v>0.018</v>
       </c>
       <c r="R125" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.011</v>
       </c>
       <c r="S125" t="n">
         <v>0</v>
       </c>
       <c r="T125" t="n">
-        <v>-0.047</v>
+        <v>-0.059</v>
       </c>
     </row>
     <row r="126">
@@ -9239,13 +9239,13 @@
         <v>-25</v>
       </c>
       <c r="J126" t="n">
-        <v>9355</v>
+        <v>9867</v>
       </c>
       <c r="K126" t="n">
         <v>6936</v>
       </c>
       <c r="L126" t="n">
-        <v>0.1132901171875</v>
+        <v>0.11133701171875</v>
       </c>
       <c r="M126" t="b">
         <v>0</v>
@@ -9309,13 +9309,13 @@
         <v>0</v>
       </c>
       <c r="J127" t="n">
-        <v>6903</v>
+        <v>7214</v>
       </c>
       <c r="K127" t="n">
         <v>21998</v>
       </c>
       <c r="L127" t="n">
-        <v>0.11914943359375</v>
+        <v>0.116219775390625</v>
       </c>
       <c r="M127" t="b">
         <v>0</v>
@@ -9331,7 +9331,7 @@
         </is>
       </c>
       <c r="P127" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="Q127" t="n">
         <v>0.004</v>
@@ -9343,7 +9343,7 @@
         <v>0</v>
       </c>
       <c r="T127" t="n">
-        <v>-0.015</v>
+        <v>-0.014</v>
       </c>
     </row>
     <row r="128">
@@ -9364,7 +9364,7 @@
         <v>446</v>
       </c>
       <c r="E128" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="F128" t="n">
         <v>0.02</v>
@@ -9373,19 +9373,19 @@
         <v>0.03</v>
       </c>
       <c r="H128" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="I128" t="n">
-        <v>0</v>
+        <v>-33.333336</v>
       </c>
       <c r="J128" t="n">
-        <v>4058</v>
+        <v>4220</v>
       </c>
       <c r="K128" t="n">
         <v>6800</v>
       </c>
       <c r="L128" t="n">
-        <v>0.125985302734375</v>
+        <v>0.124032197265625</v>
       </c>
       <c r="M128" t="b">
         <v>0</v>
@@ -9449,13 +9449,13 @@
         <v>0</v>
       </c>
       <c r="J129" t="n">
-        <v>1169</v>
+        <v>1722</v>
       </c>
       <c r="K129" t="n">
         <v>5261</v>
       </c>
       <c r="L129" t="n">
-        <v>0.13086806640625</v>
+        <v>0.1289149609375</v>
       </c>
       <c r="M129" t="b">
         <v>0</v>
@@ -9504,7 +9504,7 @@
         <v>448</v>
       </c>
       <c r="E130" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="F130" t="n">
         <v>0.01</v>
@@ -9513,19 +9513,19 @@
         <v>0.02</v>
       </c>
       <c r="H130" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="I130" t="n">
-        <v>-50</v>
+        <v>0</v>
       </c>
       <c r="J130" t="n">
-        <v>1263</v>
+        <v>1414</v>
       </c>
       <c r="K130" t="n">
         <v>5857</v>
       </c>
       <c r="L130" t="n">
-        <v>0.14258669921875</v>
+        <v>0.14063359375</v>
       </c>
       <c r="M130" t="b">
         <v>0</v>
@@ -9589,7 +9589,7 @@
         <v>-50</v>
       </c>
       <c r="J131" t="n">
-        <v>1578</v>
+        <v>1829</v>
       </c>
       <c r="K131" t="n">
         <v>4764</v>
@@ -9623,7 +9623,7 @@
         <v>0</v>
       </c>
       <c r="T131" t="n">
-        <v>-0.001</v>
+        <v>-0.002</v>
       </c>
     </row>
     <row r="132">
@@ -9659,13 +9659,13 @@
         <v>0</v>
       </c>
       <c r="J132" t="n">
-        <v>1494</v>
+        <v>1512</v>
       </c>
       <c r="K132" t="n">
         <v>34672</v>
       </c>
       <c r="L132" t="n">
-        <v>0.1523522265625</v>
+        <v>0.148446015625</v>
       </c>
       <c r="M132" t="b">
         <v>0</v>
@@ -9693,7 +9693,7 @@
         <v>0</v>
       </c>
       <c r="T132" t="n">
-        <v>-0.002</v>
+        <v>-0.001</v>
       </c>
     </row>
     <row r="133">
@@ -9735,7 +9735,7 @@
         <v>8782</v>
       </c>
       <c r="L133" t="n">
-        <v>0.164070859375</v>
+        <v>0.1601646484375</v>
       </c>
       <c r="M133" t="b">
         <v>0</v>
@@ -9763,7 +9763,7 @@
         <v>0</v>
       </c>
       <c r="T133" t="n">
-        <v>-0.002</v>
+        <v>-0.001</v>
       </c>
     </row>
     <row r="134">
@@ -9875,7 +9875,7 @@
         <v>1589</v>
       </c>
       <c r="L135" t="n">
-        <v>0.1836019140625</v>
+        <v>0.179695703125</v>
       </c>
       <c r="M135" t="b">
         <v>0</v>
@@ -9945,7 +9945,7 @@
         <v>2946</v>
       </c>
       <c r="L136" t="n">
-        <v>0.195320546875</v>
+        <v>0.1914143359375</v>
       </c>
       <c r="M136" t="b">
         <v>0</v>
@@ -10085,7 +10085,7 @@
         <v>4161</v>
       </c>
       <c r="L138" t="n">
-        <v>0.2148516015625</v>
+        <v>0.210945390625</v>
       </c>
       <c r="M138" t="b">
         <v>0</v>
@@ -10359,13 +10359,13 @@
         <v>0</v>
       </c>
       <c r="J142" t="n">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="K142" t="n">
         <v>70387</v>
       </c>
       <c r="L142" t="n">
-        <v>0.2539137109375</v>
+        <v>0.2500075</v>
       </c>
       <c r="M142" t="b">
         <v>0</v>
@@ -10505,7 +10505,7 @@
         <v>2740</v>
       </c>
       <c r="L144" t="n">
-        <v>0.2929758203124999</v>
+        <v>0.2890696093749999</v>
       </c>
       <c r="M144" t="b">
         <v>0</v>
@@ -10575,7 +10575,7 @@
         <v>4514</v>
       </c>
       <c r="L145" t="n">
-        <v>0.304694453125</v>
+        <v>0.3007882421875</v>
       </c>
       <c r="M145" t="b">
         <v>0</v>
@@ -10785,7 +10785,7 @@
         <v>12025</v>
       </c>
       <c r="L148" t="n">
-        <v>0.3515689843749999</v>
+        <v>0.3476627734375</v>
       </c>
       <c r="M148" t="b">
         <v>0</v>
@@ -10925,7 +10925,7 @@
         <v>267</v>
       </c>
       <c r="L150" t="n">
-        <v>0.3867248828124999</v>
+        <v>0.382818671875</v>
       </c>
       <c r="M150" t="b">
         <v>0</v>
@@ -10995,7 +10995,7 @@
         <v>5838</v>
       </c>
       <c r="L151" t="n">
-        <v>0.398443515625</v>
+        <v>0.39063109375</v>
       </c>
       <c r="M151" t="b">
         <v>0</v>
@@ -11763,7 +11763,7 @@
         <v>1069</v>
       </c>
       <c r="L162" t="n">
-        <v>0.73437765625</v>
+        <v>0.7187528125</v>
       </c>
       <c r="M162" t="b">
         <v>0</v>
@@ -11903,7 +11903,7 @@
         <v>688</v>
       </c>
       <c r="L164" t="n">
-        <v>0.851563984375</v>
+        <v>0.8437515624999999</v>
       </c>
       <c r="M164" t="b">
         <v>0</v>

</xml_diff>